<commit_message>
Changed end date formula
</commit_message>
<xml_diff>
--- a/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
+++ b/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Managing Multiple Project Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED219B0-B056-D44A-A179-AE9DE000F64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013083E3-B579-D94A-BACE-99C649767DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" activeTab="1" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="3" r:id="rId1"/>
@@ -205,6 +205,9 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
+      <numFmt numFmtId="19" formatCode="d/m/yy"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
@@ -230,9 +233,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="d/mm/yyyy"/>
@@ -321,15 +321,15 @@
     <tableColumn id="3" xr3:uid="{13477DA8-3E2B-9140-828B-5E4EEC4B192E}" name="Manager"/>
     <tableColumn id="4" xr3:uid="{6F6235F3-DCA0-BE4A-80AD-F124C1F29DF7}" name="Start Date" dataDxfId="5"/>
     <tableColumn id="5" xr3:uid="{906D9425-A9AF-D946-BD7E-AABF37A5C06F}" name="Duration"/>
-    <tableColumn id="9" xr3:uid="{49251E86-4677-9C41-8F83-14B60BE792A2}" name="End Date" dataDxfId="4">
-      <calculatedColumnFormula>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</calculatedColumnFormula>
+    <tableColumn id="9" xr3:uid="{49251E86-4677-9C41-8F83-14B60BE792A2}" name="End Date" dataDxfId="0">
+      <calculatedColumnFormula>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5410ED6D-ABC2-B749-B761-98A3ACF6E8B5}" name="Days completed" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{1E1A1903-5E63-2C42-A785-7622E4CE1FFD}" name="Progress" dataDxfId="2">
+    <tableColumn id="10" xr3:uid="{5410ED6D-ABC2-B749-B761-98A3ACF6E8B5}" name="Days completed" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{1E1A1903-5E63-2C42-A785-7622E4CE1FFD}" name="Progress" dataDxfId="3">
       <calculatedColumnFormula>Table1[[#This Row],[Days completed]]/Table1[[#This Row],[Duration]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5529251C-746B-0F49-8B21-221411C8E693}" name="Budget" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{2781FA1C-8107-3A45-8365-873CEB86F752}" name="Actual" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{5529251C-746B-0F49-8B21-221411C8E693}" name="Budget" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{2781FA1C-8107-3A45-8365-873CEB86F752}" name="Actual" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -634,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18BA6329-E680-5548-BB82-D6FB67EB7003}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -659,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97670974-E5A2-664C-82DE-A6BD35D73425}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,8 +714,8 @@
         <v>5</v>
       </c>
       <c r="F2" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
-        <v>43882</v>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
+        <v>43884</v>
       </c>
       <c r="G2" s="3">
         <v>2</v>
@@ -748,7 +748,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43885</v>
       </c>
       <c r="G3" s="3">
@@ -782,7 +782,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43892</v>
       </c>
       <c r="G4" s="3">
@@ -816,7 +816,7 @@
         <v>9</v>
       </c>
       <c r="F5" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43894</v>
       </c>
       <c r="G5" s="3">
@@ -850,7 +850,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43881</v>
       </c>
       <c r="G6" s="3">
@@ -884,7 +884,7 @@
         <v>6</v>
       </c>
       <c r="F7" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43888</v>
       </c>
       <c r="G7" s="3">
@@ -918,8 +918,8 @@
         <v>7</v>
       </c>
       <c r="F8" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
-        <v>43889</v>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
+        <v>43891</v>
       </c>
       <c r="G8" s="3">
         <v>3</v>
@@ -952,8 +952,8 @@
         <v>5</v>
       </c>
       <c r="F9" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
-        <v>43889</v>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
+        <v>43891</v>
       </c>
       <c r="G9" s="3">
         <v>2</v>
@@ -986,7 +986,7 @@
         <v>9</v>
       </c>
       <c r="F10" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43895</v>
       </c>
       <c r="G10" s="3">
@@ -1020,7 +1020,7 @@
         <v>6</v>
       </c>
       <c r="F11" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43892</v>
       </c>
       <c r="G11" s="3">
@@ -1054,7 +1054,7 @@
         <v>7</v>
       </c>
       <c r="F12" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43887</v>
       </c>
       <c r="G12" s="3">
@@ -1088,7 +1088,7 @@
         <v>9</v>
       </c>
       <c r="F13" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43888</v>
       </c>
       <c r="G13" s="3">
@@ -1122,7 +1122,7 @@
         <v>8</v>
       </c>
       <c r="F14" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43888</v>
       </c>
       <c r="G14" s="3">
@@ -1156,8 +1156,8 @@
         <v>7</v>
       </c>
       <c r="F15" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
-        <v>43889</v>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
+        <v>43891</v>
       </c>
       <c r="G15" s="3">
         <v>3</v>
@@ -1190,7 +1190,7 @@
         <v>4</v>
       </c>
       <c r="F16" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43887</v>
       </c>
       <c r="G16" s="3">
@@ -1224,8 +1224,8 @@
         <v>6</v>
       </c>
       <c r="F17" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
-        <v>43889</v>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
+        <v>43891</v>
       </c>
       <c r="G17" s="3">
         <v>3</v>
@@ -1258,7 +1258,7 @@
         <v>6</v>
       </c>
       <c r="F18" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43892</v>
       </c>
       <c r="G18" s="3">
@@ -1292,8 +1292,8 @@
         <v>4</v>
       </c>
       <c r="F19" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
-        <v>43889</v>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
+        <v>43891</v>
       </c>
       <c r="G19" s="3">
         <v>1</v>
@@ -1326,8 +1326,8 @@
         <v>7</v>
       </c>
       <c r="F20" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
-        <v>43896</v>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
+        <v>43898</v>
       </c>
       <c r="G20" s="3">
         <v>3</v>
@@ -1360,7 +1360,7 @@
         <v>3</v>
       </c>
       <c r="F21" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43880</v>
       </c>
       <c r="G21" s="3">
@@ -1394,8 +1394,8 @@
         <v>10</v>
       </c>
       <c r="F22" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
-        <v>43889</v>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
+        <v>43891</v>
       </c>
       <c r="G22" s="3">
         <v>5</v>
@@ -1428,7 +1428,7 @@
         <v>5</v>
       </c>
       <c r="F23" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43888</v>
       </c>
       <c r="G23" s="3">
@@ -1462,7 +1462,7 @@
         <v>7</v>
       </c>
       <c r="F24" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43893</v>
       </c>
       <c r="G24" s="3">
@@ -1496,7 +1496,7 @@
         <v>7</v>
       </c>
       <c r="F25" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43895</v>
       </c>
       <c r="G25" s="3">
@@ -1530,7 +1530,7 @@
         <v>3</v>
       </c>
       <c r="F26" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43893</v>
       </c>
       <c r="G26" s="3">
@@ -1564,7 +1564,7 @@
         <v>9</v>
       </c>
       <c r="F27" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43902</v>
       </c>
       <c r="G27" s="3">
@@ -1598,8 +1598,8 @@
         <v>10</v>
       </c>
       <c r="F28" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
-        <v>43903</v>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
+        <v>43905</v>
       </c>
       <c r="G28" s="3">
         <v>2</v>
@@ -1632,7 +1632,7 @@
         <v>4</v>
       </c>
       <c r="F29" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43881</v>
       </c>
       <c r="G29" s="3">
@@ -1666,8 +1666,8 @@
         <v>8</v>
       </c>
       <c r="F30" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
-        <v>43889</v>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
+        <v>43891</v>
       </c>
       <c r="G30" s="3">
         <v>5</v>
@@ -1700,8 +1700,8 @@
         <v>10</v>
       </c>
       <c r="F31" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
-        <v>43896</v>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
+        <v>43898</v>
       </c>
       <c r="G31" s="3">
         <v>3</v>
@@ -1734,7 +1734,7 @@
         <v>6</v>
       </c>
       <c r="F32" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43893</v>
       </c>
       <c r="G32" s="3">
@@ -1768,8 +1768,8 @@
         <v>4</v>
       </c>
       <c r="F33" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
-        <v>43889</v>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
+        <v>43891</v>
       </c>
       <c r="G33" s="3">
         <v>2</v>
@@ -1802,7 +1802,7 @@
         <v>8</v>
       </c>
       <c r="F34" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43900</v>
       </c>
       <c r="G34" s="3">
@@ -1836,7 +1836,7 @@
         <v>9</v>
       </c>
       <c r="F35" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43902</v>
       </c>
       <c r="G35" s="3">
@@ -1870,7 +1870,7 @@
         <v>5</v>
       </c>
       <c r="F36" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43887</v>
       </c>
       <c r="G36" s="3">
@@ -1904,8 +1904,8 @@
         <v>3</v>
       </c>
       <c r="F37" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
-        <v>43882</v>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
+        <v>43884</v>
       </c>
       <c r="G37" s="3">
         <v>3</v>
@@ -1938,7 +1938,7 @@
         <v>7</v>
       </c>
       <c r="F38" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43892</v>
       </c>
       <c r="G38" s="3">
@@ -1972,8 +1972,8 @@
         <v>10</v>
       </c>
       <c r="F39" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
-        <v>43896</v>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
+        <v>43898</v>
       </c>
       <c r="G39" s="3">
         <v>2</v>
@@ -2006,8 +2006,8 @@
         <v>10</v>
       </c>
       <c r="F40" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
-        <v>43896</v>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
+        <v>43898</v>
       </c>
       <c r="G40" s="3">
         <v>3</v>
@@ -2040,7 +2040,7 @@
         <v>3</v>
       </c>
       <c r="F41" s="2">
-        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</f>
+        <f>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],7)</f>
         <v>43887</v>
       </c>
       <c r="G41" s="3">

</xml_diff>

<commit_message>
Removed +/- buttons and subtotal
</commit_message>
<xml_diff>
--- a/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
+++ b/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Managing Multiple Project Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2A13B8-6703-DD4D-AC67-EA4DF7EE1CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3D179F-0D14-D244-ACD9-85A1ED68AA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12880" yWindow="760" windowWidth="17360" windowHeight="17420" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="37">
   <si>
     <t>Project</t>
   </si>
@@ -150,66 +150,6 @@
   </si>
   <si>
     <t>Sum of Actual</t>
-  </si>
-  <si>
-    <t>McFay Total</t>
-  </si>
-  <si>
-    <t>Task 1 Total</t>
-  </si>
-  <si>
-    <t>Wood Total</t>
-  </si>
-  <si>
-    <t>Task 2 Total</t>
-  </si>
-  <si>
-    <t>Ladd Total</t>
-  </si>
-  <si>
-    <t>Task 3 Total</t>
-  </si>
-  <si>
-    <t>Hirsch Total</t>
-  </si>
-  <si>
-    <t>Task 4 Total</t>
-  </si>
-  <si>
-    <t>Samora Total</t>
-  </si>
-  <si>
-    <t>Task 5 Total</t>
-  </si>
-  <si>
-    <t>Task 6 Total</t>
-  </si>
-  <si>
-    <t>Task 7 Total</t>
-  </si>
-  <si>
-    <t>Task 8 Total</t>
-  </si>
-  <si>
-    <t>Alpha Total</t>
-  </si>
-  <si>
-    <t>Delta Total</t>
-  </si>
-  <si>
-    <t>Task 10 Total</t>
-  </si>
-  <si>
-    <t>Task 9 Total</t>
-  </si>
-  <si>
-    <t>Gemini Total</t>
-  </si>
-  <si>
-    <t>Orion Total</t>
-  </si>
-  <si>
-    <t>Vega Total</t>
   </si>
   <si>
     <t>Months</t>
@@ -1409,21 +1349,20 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{49A324D7-DAC3-AE4C-8B42-860D7EF2D1B0}" name="PivotTable2" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="A5:K131" firstHeaderRow="0" firstDataRow="1" firstDataCol="9"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{49A324D7-DAC3-AE4C-8B42-860D7EF2D1B0}" name="PivotTable2" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="A5:K46" firstHeaderRow="0" firstDataRow="1" firstDataCol="9"/>
   <pivotFields count="11">
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="6">
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="5">
         <item x="4"/>
         <item x="3"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
-        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="11">
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="10">
         <item x="0"/>
         <item x="9"/>
         <item x="1"/>
@@ -1434,21 +1373,19 @@
         <item x="6"/>
         <item x="7"/>
         <item x="8"/>
-        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="6">
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="5">
         <item x="0"/>
         <item x="4"/>
         <item x="2"/>
         <item x="1"/>
         <item x="3"/>
-        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" compact="0" numFmtId="14" outline="0" showAll="0">
-      <items count="12">
+    <pivotField axis="axisRow" compact="0" numFmtId="14" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="11">
         <item x="0"/>
         <item x="1"/>
         <item x="10"/>
@@ -1460,11 +1397,10 @@
         <item x="6"/>
         <item x="8"/>
         <item x="9"/>
-        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="9">
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="8">
         <item x="7"/>
         <item x="4"/>
         <item x="0"/>
@@ -1473,11 +1409,10 @@
         <item x="6"/>
         <item x="3"/>
         <item x="2"/>
-        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" compact="0" numFmtId="14" outline="0" showAll="0">
-      <items count="369">
+    <pivotField axis="axisRow" compact="0" numFmtId="14" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="368">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -1846,11 +1781,10 @@
         <item x="365"/>
         <item x="366"/>
         <item x="367"/>
-        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" compact="0" numFmtId="3" outline="0" showAll="0">
-      <items count="9">
+    <pivotField axis="axisRow" compact="0" numFmtId="3" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="8">
         <item x="4"/>
         <item x="3"/>
         <item x="0"/>
@@ -1859,11 +1793,10 @@
         <item x="6"/>
         <item x="5"/>
         <item x="7"/>
-        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" compact="0" numFmtId="9" outline="0" showAll="0">
-      <items count="20">
+    <pivotField axis="axisRow" compact="0" numFmtId="9" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="19">
         <item x="4"/>
         <item x="6"/>
         <item x="14"/>
@@ -1883,13 +1816,12 @@
         <item x="9"/>
         <item x="13"/>
         <item x="7"/>
-        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" compact="0" numFmtId="3" outline="0" showAll="0"/>
-    <pivotField dataField="1" compact="0" numFmtId="3" outline="0" showAll="0"/>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="15">
+    <pivotField dataField="1" compact="0" numFmtId="3" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="3" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="14">
         <item sd="0" x="0"/>
         <item sd="0" x="1"/>
         <item sd="0" x="2"/>
@@ -1904,7 +1836,6 @@
         <item sd="0" x="11"/>
         <item sd="0" x="12"/>
         <item sd="0" x="13"/>
-        <item t="default"/>
       </items>
     </pivotField>
   </pivotFields>
@@ -1919,98 +1850,47 @@
     <field x="6"/>
     <field x="7"/>
   </rowFields>
-  <rowItems count="126">
+  <rowItems count="41">
     <i>
       <x/>
       <x/>
       <x v="2"/>
       <x v="3"/>
     </i>
-    <i t="default" r="2">
-      <x v="2"/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
     <i r="1">
       <x v="2"/>
       <x v="4"/>
       <x v="3"/>
-    </i>
-    <i t="default" r="2">
-      <x v="4"/>
-    </i>
-    <i t="default" r="1">
-      <x v="2"/>
     </i>
     <i r="1">
       <x v="3"/>
       <x v="1"/>
       <x v="2"/>
     </i>
-    <i t="default" r="2">
-      <x v="1"/>
-    </i>
-    <i t="default" r="1">
-      <x v="3"/>
-    </i>
     <i r="1">
       <x v="4"/>
       <x/>
       <x v="2"/>
-    </i>
-    <i t="default" r="2">
-      <x/>
-    </i>
-    <i t="default" r="1">
-      <x v="4"/>
     </i>
     <i r="1">
       <x v="5"/>
       <x v="3"/>
       <x v="3"/>
     </i>
-    <i t="default" r="2">
-      <x v="3"/>
-    </i>
-    <i t="default" r="1">
-      <x v="5"/>
-    </i>
     <i r="1">
       <x v="6"/>
       <x v="2"/>
       <x v="3"/>
-    </i>
-    <i t="default" r="2">
-      <x v="2"/>
-    </i>
-    <i t="default" r="1">
-      <x v="6"/>
     </i>
     <i r="1">
       <x v="7"/>
       <x v="4"/>
       <x v="3"/>
     </i>
-    <i t="default" r="2">
-      <x v="4"/>
-    </i>
-    <i t="default" r="1">
-      <x v="7"/>
-    </i>
     <i r="1">
       <x v="8"/>
       <x v="1"/>
       <x v="2"/>
-    </i>
-    <i t="default" r="2">
-      <x v="1"/>
-    </i>
-    <i t="default" r="1">
-      <x v="8"/>
-    </i>
-    <i t="default">
-      <x/>
     </i>
     <i>
       <x v="1"/>
@@ -2018,32 +1898,55 @@
       <x/>
       <x v="3"/>
     </i>
-    <i t="default" r="2">
-      <x/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
     <i r="1">
       <x v="2"/>
       <x v="3"/>
       <x v="3"/>
-    </i>
-    <i t="default" r="2">
-      <x v="3"/>
-    </i>
-    <i t="default" r="1">
-      <x v="2"/>
     </i>
     <i r="1">
       <x v="3"/>
       <x v="2"/>
       <x v="2"/>
     </i>
-    <i t="default" r="2">
+    <i r="1">
+      <x v="4"/>
+      <x v="4"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+      <x/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+      <x v="3"/>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+      <x/>
       <x v="2"/>
     </i>
-    <i t="default" r="1">
+    <i r="1">
+      <x v="1"/>
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x v="3"/>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+      <x v="2"/>
       <x v="3"/>
     </i>
     <i r="1">
@@ -2051,161 +1954,30 @@
       <x v="4"/>
       <x v="3"/>
     </i>
-    <i t="default" r="2">
-      <x v="4"/>
-    </i>
-    <i t="default" r="1">
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-      <x v="1"/>
-      <x v="3"/>
-    </i>
-    <i t="default" r="2">
-      <x v="1"/>
-    </i>
-    <i t="default" r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-      <x/>
-      <x v="3"/>
-    </i>
-    <i t="default" r="2">
-      <x/>
-    </i>
-    <i t="default" r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-      <x v="3"/>
-      <x v="3"/>
-    </i>
-    <i t="default" r="2">
-      <x v="3"/>
-    </i>
-    <i t="default" r="1">
-      <x v="7"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x/>
-      <x/>
-      <x v="2"/>
-    </i>
-    <i t="default" r="2">
-      <x/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-      <x v="1"/>
-      <x v="3"/>
-    </i>
-    <i t="default" r="2">
-      <x v="1"/>
-    </i>
-    <i t="default" r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-      <x v="3"/>
-      <x v="2"/>
-    </i>
-    <i t="default" r="2">
-      <x v="3"/>
-    </i>
-    <i t="default" r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-      <x v="2"/>
-      <x v="3"/>
-    </i>
-    <i t="default" r="2">
-      <x v="2"/>
-    </i>
-    <i t="default" r="1">
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="4"/>
-      <x v="4"/>
-      <x v="3"/>
-    </i>
-    <i t="default" r="2">
-      <x v="4"/>
-    </i>
-    <i t="default" r="1">
-      <x v="4"/>
-    </i>
     <i r="1">
       <x v="5"/>
       <x v="1"/>
       <x v="2"/>
-    </i>
-    <i t="default" r="2">
-      <x v="1"/>
-    </i>
-    <i t="default" r="1">
-      <x v="5"/>
     </i>
     <i r="1">
       <x v="6"/>
       <x/>
       <x v="2"/>
     </i>
-    <i t="default" r="2">
-      <x/>
-    </i>
-    <i t="default" r="1">
-      <x v="6"/>
-    </i>
     <i r="1">
       <x v="7"/>
       <x v="3"/>
       <x v="2"/>
-    </i>
-    <i t="default" r="2">
-      <x v="3"/>
-    </i>
-    <i t="default" r="1">
-      <x v="7"/>
     </i>
     <i r="1">
       <x v="8"/>
       <x v="2"/>
       <x v="3"/>
     </i>
-    <i t="default" r="2">
-      <x v="2"/>
-    </i>
-    <i t="default" r="1">
-      <x v="8"/>
-    </i>
     <i r="1">
       <x v="9"/>
       <x v="4"/>
       <x v="3"/>
-    </i>
-    <i t="default" r="2">
-      <x v="4"/>
-    </i>
-    <i t="default" r="1">
-      <x v="9"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
     </i>
     <i>
       <x v="3"/>
@@ -2213,43 +1985,19 @@
       <x/>
       <x v="2"/>
     </i>
-    <i t="default" r="2">
-      <x/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
     <i r="1">
       <x v="1"/>
       <x v="1"/>
       <x v="2"/>
-    </i>
-    <i t="default" r="2">
-      <x v="1"/>
-    </i>
-    <i t="default" r="1">
-      <x v="1"/>
     </i>
     <i r="1">
       <x v="2"/>
       <x v="3"/>
       <x v="3"/>
     </i>
-    <i t="default" r="2">
-      <x v="3"/>
-    </i>
-    <i t="default" r="1">
-      <x v="2"/>
-    </i>
     <i r="1">
       <x v="3"/>
       <x v="2"/>
-      <x v="3"/>
-    </i>
-    <i t="default" r="2">
-      <x v="2"/>
-    </i>
-    <i t="default" r="1">
       <x v="3"/>
     </i>
     <i r="1">
@@ -2257,68 +2005,29 @@
       <x v="4"/>
       <x v="2"/>
     </i>
-    <i t="default" r="2">
-      <x v="4"/>
-    </i>
-    <i t="default" r="1">
-      <x v="4"/>
-    </i>
     <i r="1">
       <x v="5"/>
       <x v="1"/>
       <x v="2"/>
-    </i>
-    <i t="default" r="2">
-      <x v="1"/>
-    </i>
-    <i t="default" r="1">
-      <x v="5"/>
     </i>
     <i r="1">
       <x v="6"/>
       <x/>
       <x v="2"/>
     </i>
-    <i t="default" r="2">
-      <x/>
-    </i>
-    <i t="default" r="1">
-      <x v="6"/>
-    </i>
     <i r="1">
       <x v="7"/>
       <x v="3"/>
       <x v="3"/>
-    </i>
-    <i t="default" r="2">
-      <x v="3"/>
-    </i>
-    <i t="default" r="1">
-      <x v="7"/>
     </i>
     <i r="1">
       <x v="8"/>
       <x v="2"/>
       <x v="3"/>
     </i>
-    <i t="default" r="2">
-      <x v="2"/>
-    </i>
-    <i t="default" r="1">
-      <x v="8"/>
-    </i>
     <i r="1">
       <x v="9"/>
       <x v="4"/>
-      <x v="3"/>
-    </i>
-    <i t="default" r="2">
-      <x v="4"/>
-    </i>
-    <i t="default" r="1">
-      <x v="9"/>
-    </i>
-    <i t="default">
       <x v="3"/>
     </i>
     <i>
@@ -2327,21 +2036,9 @@
       <x/>
       <x v="3"/>
     </i>
-    <i t="default" r="2">
-      <x/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
     <i r="1">
       <x v="2"/>
       <x v="3"/>
-      <x v="2"/>
-    </i>
-    <i t="default" r="2">
-      <x v="3"/>
-    </i>
-    <i t="default" r="1">
       <x v="2"/>
     </i>
     <i r="1">
@@ -2349,36 +2046,15 @@
       <x v="2"/>
       <x v="3"/>
     </i>
-    <i t="default" r="2">
-      <x v="2"/>
-    </i>
-    <i t="default" r="1">
-      <x v="3"/>
-    </i>
     <i r="1">
       <x v="4"/>
       <x v="4"/>
       <x v="3"/>
     </i>
-    <i t="default" r="2">
-      <x v="4"/>
-    </i>
-    <i t="default" r="1">
-      <x v="4"/>
-    </i>
     <i r="1">
       <x v="5"/>
       <x v="1"/>
       <x v="3"/>
-    </i>
-    <i t="default" r="2">
-      <x v="1"/>
-    </i>
-    <i t="default" r="1">
-      <x v="5"/>
-    </i>
-    <i t="default">
-      <x v="4"/>
     </i>
     <i t="grand">
       <x/>
@@ -2405,7 +2081,7 @@
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
     <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
     </ext>
   </extLst>
 </pivotTableDefinition>
@@ -2731,10 +2407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18BA6329-E680-5548-BB82-D6FB67EB7003}">
-  <dimension ref="A1:K131"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2763,7 +2439,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>3</v>
@@ -2808,142 +2484,193 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
       </c>
       <c r="J7" s="7">
-        <v>96000</v>
+        <v>513000</v>
       </c>
       <c r="K7" s="7">
-        <v>32256</v>
+        <v>226233</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>37</v>
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
       </c>
       <c r="J8" s="7">
-        <v>96000</v>
+        <v>616000</v>
       </c>
       <c r="K8" s="7">
-        <v>32256</v>
+        <v>401579</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="7">
+        <v>817000</v>
+      </c>
+      <c r="K9" s="7">
+        <v>807069</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="J9" s="7">
-        <v>513000</v>
-      </c>
-      <c r="K9" s="7">
-        <v>226233</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
-        <v>38</v>
-      </c>
       <c r="J10" s="7">
-        <v>513000</v>
+        <v>372000</v>
       </c>
       <c r="K10" s="7">
-        <v>226233</v>
+        <v>173166</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>39</v>
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
       </c>
       <c r="J11" s="7">
-        <v>513000</v>
+        <v>50000</v>
       </c>
       <c r="K11" s="7">
-        <v>226233</v>
+        <v>8400</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" s="7">
+        <v>807000</v>
+      </c>
+      <c r="K12" s="7">
+        <v>262679</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
         <v>20</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>33</v>
       </c>
-      <c r="J12" s="7">
-        <v>616000</v>
-      </c>
-      <c r="K12" s="7">
-        <v>401579</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
-        <v>40</v>
-      </c>
       <c r="J13" s="7">
-        <v>616000</v>
+        <v>691000</v>
       </c>
       <c r="K13" s="7">
-        <v>401579</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
       </c>
       <c r="J14" s="7">
-        <v>616000</v>
+        <v>787000</v>
       </c>
       <c r="K14" s="7">
-        <v>401579</v>
+        <v>727188</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D15" t="s">
+        <v>32</v>
+      </c>
+      <c r="J15" s="7">
+        <v>228000</v>
+      </c>
+      <c r="K15" s="7">
+        <v>47880</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
         <v>33</v>
       </c>
-      <c r="J15" s="7">
-        <v>817000</v>
-      </c>
-      <c r="K15" s="7">
-        <v>807069</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
-        <v>42</v>
-      </c>
       <c r="J16" s="7">
-        <v>817000</v>
+        <v>147000</v>
       </c>
       <c r="K16" s="7">
-        <v>807069</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>43</v>
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>32</v>
       </c>
       <c r="J17" s="7">
-        <v>817000</v>
+        <v>338000</v>
       </c>
       <c r="K17" s="7">
-        <v>807069</v>
+        <v>205123</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -2951,171 +2678,228 @@
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D18" t="s">
         <v>32</v>
       </c>
       <c r="J18" s="7">
-        <v>372000</v>
+        <v>857000</v>
       </c>
       <c r="K18" s="7">
-        <v>173166</v>
+        <v>305949</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
+        <v>32</v>
       </c>
       <c r="J19" s="7">
-        <v>372000</v>
+        <v>602000</v>
       </c>
       <c r="K19" s="7">
-        <v>173166</v>
+        <v>322371</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>45</v>
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>32</v>
       </c>
       <c r="J20" s="7">
-        <v>372000</v>
+        <v>990000</v>
       </c>
       <c r="K20" s="7">
-        <v>173166</v>
+        <v>451440</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J21" s="7">
+        <v>218000</v>
+      </c>
+      <c r="K21" s="7">
+        <v>97337</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" t="s">
         <v>32</v>
       </c>
-      <c r="J21" s="7">
-        <v>50000</v>
-      </c>
-      <c r="K21" s="7">
-        <v>8400</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C22" t="s">
-        <v>36</v>
-      </c>
       <c r="J22" s="7">
-        <v>50000</v>
+        <v>416000</v>
       </c>
       <c r="K22" s="7">
-        <v>8400</v>
+        <v>175015</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>46</v>
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" t="s">
+        <v>33</v>
       </c>
       <c r="J23" s="7">
-        <v>50000</v>
+        <v>393000</v>
       </c>
       <c r="K23" s="7">
-        <v>8400</v>
+        <v>177440</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D24" t="s">
         <v>32</v>
       </c>
       <c r="J24" s="7">
-        <v>807000</v>
+        <v>86000</v>
       </c>
       <c r="K24" s="7">
-        <v>262679</v>
+        <v>31046</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>18</v>
+      </c>
+      <c r="D25" t="s">
+        <v>32</v>
       </c>
       <c r="J25" s="7">
-        <v>807000</v>
+        <v>732000</v>
       </c>
       <c r="K25" s="7">
-        <v>262679</v>
+        <v>261324</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>47</v>
+        <v>19</v>
+      </c>
+      <c r="C26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" t="s">
+        <v>33</v>
       </c>
       <c r="J26" s="7">
-        <v>807000</v>
+        <v>492000</v>
       </c>
       <c r="K26" s="7">
-        <v>262679</v>
+        <v>116850</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C27" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D27" t="s">
         <v>33</v>
       </c>
       <c r="J27" s="7">
-        <v>691000</v>
+        <v>188000</v>
       </c>
       <c r="K27" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>14</v>
+      </c>
+      <c r="D28" t="s">
+        <v>33</v>
       </c>
       <c r="J28" s="7">
-        <v>691000</v>
+        <v>180000</v>
       </c>
       <c r="K28" s="7">
-        <v>0</v>
+        <v>79380</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>48</v>
+        <v>23</v>
+      </c>
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" t="s">
+        <v>32</v>
       </c>
       <c r="J29" s="7">
-        <v>691000</v>
+        <v>582000</v>
       </c>
       <c r="K29" s="7">
-        <v>0</v>
+        <v>195231</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>49</v>
+      <c r="B30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" t="s">
+        <v>32</v>
       </c>
       <c r="J30" s="7">
-        <v>3962000</v>
+        <v>562000</v>
       </c>
       <c r="K30" s="7">
-        <v>1911382</v>
+        <v>74746</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B31" t="s">
         <v>11</v>
@@ -3124,118 +2908,154 @@
         <v>12</v>
       </c>
       <c r="D31" t="s">
+        <v>33</v>
+      </c>
+      <c r="J31" s="7">
+        <v>293000</v>
+      </c>
+      <c r="K31" s="7">
+        <v>273001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" t="s">
+        <v>33</v>
+      </c>
+      <c r="J32" s="7">
+        <v>68000</v>
+      </c>
+      <c r="K32" s="7">
+        <v>64987</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" t="s">
         <v>32</v>
       </c>
-      <c r="J31" s="7">
-        <v>787000</v>
-      </c>
-      <c r="K31" s="7">
-        <v>727188</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C32" t="s">
-        <v>42</v>
-      </c>
-      <c r="J32" s="7">
-        <v>787000</v>
-      </c>
-      <c r="K32" s="7">
-        <v>727188</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>37</v>
-      </c>
       <c r="J33" s="7">
-        <v>787000</v>
+        <v>224000</v>
       </c>
       <c r="K33" s="7">
-        <v>727188</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+        <v>57910</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D34" t="s">
         <v>32</v>
       </c>
       <c r="J34" s="7">
-        <v>228000</v>
+        <v>978000</v>
       </c>
       <c r="K34" s="7">
-        <v>47880</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>17</v>
+      </c>
       <c r="C35" t="s">
-        <v>44</v>
+        <v>18</v>
+      </c>
+      <c r="D35" t="s">
+        <v>33</v>
       </c>
       <c r="J35" s="7">
-        <v>228000</v>
+        <v>932000</v>
       </c>
       <c r="K35" s="7">
-        <v>47880</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
+        <v>379157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>39</v>
+        <v>19</v>
+      </c>
+      <c r="C36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" t="s">
+        <v>33</v>
       </c>
       <c r="J36" s="7">
-        <v>228000</v>
+        <v>854000</v>
       </c>
       <c r="K36" s="7">
-        <v>47880</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+        <v>322812</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C37" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D37" t="s">
         <v>33</v>
       </c>
       <c r="J37" s="7">
-        <v>147000</v>
+        <v>81000</v>
       </c>
       <c r="K37" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+        <v>38461</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>22</v>
+      </c>
       <c r="C38" t="s">
-        <v>36</v>
+        <v>14</v>
+      </c>
+      <c r="D38" t="s">
+        <v>32</v>
       </c>
       <c r="J38" s="7">
-        <v>147000</v>
+        <v>169000</v>
       </c>
       <c r="K38" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
+        <v>136468</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>41</v>
+        <v>23</v>
+      </c>
+      <c r="C39" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" t="s">
+        <v>32</v>
       </c>
       <c r="J39" s="7">
-        <v>147000</v>
+        <v>61000</v>
       </c>
       <c r="K39" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
+        <v>12078</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C40" t="s">
         <v>18</v>
@@ -3244,1187 +3064,108 @@
         <v>32</v>
       </c>
       <c r="J40" s="7">
-        <v>338000</v>
+        <v>645000</v>
       </c>
       <c r="K40" s="7">
-        <v>205123</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
+        <v>273048</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
       <c r="C41" t="s">
-        <v>38</v>
+        <v>12</v>
+      </c>
+      <c r="D41" t="s">
+        <v>32</v>
       </c>
       <c r="J41" s="7">
-        <v>338000</v>
+        <v>839000</v>
       </c>
       <c r="K41" s="7">
-        <v>205123</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
+        <v>406974</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>43</v>
+        <v>13</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" t="s">
+        <v>33</v>
       </c>
       <c r="J42" s="7">
-        <v>338000</v>
+        <v>729000</v>
       </c>
       <c r="K42" s="7">
-        <v>205123</v>
-      </c>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
+        <v>487139</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C43" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D43" t="s">
         <v>32</v>
       </c>
       <c r="J43" s="7">
-        <v>857000</v>
+        <v>826000</v>
       </c>
       <c r="K43" s="7">
-        <v>305949</v>
-      </c>
-    </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
+        <v>298186</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>17</v>
+      </c>
       <c r="C44" t="s">
-        <v>40</v>
+        <v>18</v>
+      </c>
+      <c r="D44" t="s">
+        <v>32</v>
       </c>
       <c r="J44" s="7">
-        <v>857000</v>
+        <v>895000</v>
       </c>
       <c r="K44" s="7">
-        <v>305949</v>
-      </c>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
+        <v>280583</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>45</v>
+        <v>19</v>
+      </c>
+      <c r="C45" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" t="s">
+        <v>32</v>
       </c>
       <c r="J45" s="7">
-        <v>857000</v>
+        <v>341000</v>
       </c>
       <c r="K45" s="7">
-        <v>305949</v>
-      </c>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
-        <v>21</v>
-      </c>
-      <c r="C46" t="s">
-        <v>12</v>
-      </c>
-      <c r="D46" t="s">
-        <v>32</v>
+        <v>129785</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>31</v>
       </c>
       <c r="J46" s="7">
-        <v>602000</v>
+        <v>19695000</v>
       </c>
       <c r="K46" s="7">
-        <v>322371</v>
-      </c>
-    </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C47" t="s">
-        <v>42</v>
-      </c>
-      <c r="J47" s="7">
-        <v>602000</v>
-      </c>
-      <c r="K47" s="7">
-        <v>322371</v>
-      </c>
-    </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
-        <v>46</v>
-      </c>
-      <c r="J48" s="7">
-        <v>602000</v>
-      </c>
-      <c r="K48" s="7">
-        <v>322371</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
-        <v>22</v>
-      </c>
-      <c r="C49" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49" t="s">
-        <v>32</v>
-      </c>
-      <c r="J49" s="7">
-        <v>990000</v>
-      </c>
-      <c r="K49" s="7">
-        <v>451440</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C50" t="s">
-        <v>44</v>
-      </c>
-      <c r="J50" s="7">
-        <v>990000</v>
-      </c>
-      <c r="K50" s="7">
-        <v>451440</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
-        <v>47</v>
-      </c>
-      <c r="J51" s="7">
-        <v>990000</v>
-      </c>
-      <c r="K51" s="7">
-        <v>451440</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>50</v>
-      </c>
-      <c r="J52" s="7">
-        <v>3949000</v>
-      </c>
-      <c r="K52" s="7">
-        <v>2059951</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>10</v>
-      </c>
-      <c r="B53" t="s">
-        <v>11</v>
-      </c>
-      <c r="C53" t="s">
-        <v>12</v>
-      </c>
-      <c r="D53" t="s">
-        <v>33</v>
-      </c>
-      <c r="J53" s="7">
-        <v>218000</v>
-      </c>
-      <c r="K53" s="7">
-        <v>97337</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C54" t="s">
-        <v>42</v>
-      </c>
-      <c r="J54" s="7">
-        <v>218000</v>
-      </c>
-      <c r="K54" s="7">
-        <v>97337</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B55" t="s">
-        <v>37</v>
-      </c>
-      <c r="J55" s="7">
-        <v>218000</v>
-      </c>
-      <c r="K55" s="7">
-        <v>97337</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B56" t="s">
-        <v>25</v>
-      </c>
-      <c r="C56" t="s">
-        <v>20</v>
-      </c>
-      <c r="D56" t="s">
-        <v>32</v>
-      </c>
-      <c r="J56" s="7">
-        <v>416000</v>
-      </c>
-      <c r="K56" s="7">
-        <v>175015</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C57" t="s">
-        <v>40</v>
-      </c>
-      <c r="J57" s="7">
-        <v>416000</v>
-      </c>
-      <c r="K57" s="7">
-        <v>175015</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B58" t="s">
-        <v>51</v>
-      </c>
-      <c r="J58" s="7">
-        <v>416000</v>
-      </c>
-      <c r="K58" s="7">
-        <v>175015</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B59" t="s">
-        <v>13</v>
-      </c>
-      <c r="C59" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59" t="s">
-        <v>33</v>
-      </c>
-      <c r="J59" s="7">
-        <v>393000</v>
-      </c>
-      <c r="K59" s="7">
-        <v>177440</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C60" t="s">
-        <v>44</v>
-      </c>
-      <c r="J60" s="7">
-        <v>393000</v>
-      </c>
-      <c r="K60" s="7">
-        <v>177440</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B61" t="s">
-        <v>39</v>
-      </c>
-      <c r="J61" s="7">
-        <v>393000</v>
-      </c>
-      <c r="K61" s="7">
-        <v>177440</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B62" t="s">
-        <v>15</v>
-      </c>
-      <c r="C62" t="s">
-        <v>16</v>
-      </c>
-      <c r="D62" t="s">
-        <v>32</v>
-      </c>
-      <c r="J62" s="7">
-        <v>86000</v>
-      </c>
-      <c r="K62" s="7">
-        <v>31046</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C63" t="s">
-        <v>36</v>
-      </c>
-      <c r="J63" s="7">
-        <v>86000</v>
-      </c>
-      <c r="K63" s="7">
-        <v>31046</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B64" t="s">
-        <v>41</v>
-      </c>
-      <c r="J64" s="7">
-        <v>86000</v>
-      </c>
-      <c r="K64" s="7">
-        <v>31046</v>
-      </c>
-    </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B65" t="s">
-        <v>17</v>
-      </c>
-      <c r="C65" t="s">
-        <v>18</v>
-      </c>
-      <c r="D65" t="s">
-        <v>32</v>
-      </c>
-      <c r="J65" s="7">
-        <v>732000</v>
-      </c>
-      <c r="K65" s="7">
-        <v>261324</v>
-      </c>
-    </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C66" t="s">
-        <v>38</v>
-      </c>
-      <c r="J66" s="7">
-        <v>732000</v>
-      </c>
-      <c r="K66" s="7">
-        <v>261324</v>
-      </c>
-    </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B67" t="s">
-        <v>43</v>
-      </c>
-      <c r="J67" s="7">
-        <v>732000</v>
-      </c>
-      <c r="K67" s="7">
-        <v>261324</v>
-      </c>
-    </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B68" t="s">
-        <v>19</v>
-      </c>
-      <c r="C68" t="s">
-        <v>20</v>
-      </c>
-      <c r="D68" t="s">
-        <v>33</v>
-      </c>
-      <c r="J68" s="7">
-        <v>492000</v>
-      </c>
-      <c r="K68" s="7">
-        <v>116850</v>
-      </c>
-    </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C69" t="s">
-        <v>40</v>
-      </c>
-      <c r="J69" s="7">
-        <v>492000</v>
-      </c>
-      <c r="K69" s="7">
-        <v>116850</v>
-      </c>
-    </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B70" t="s">
-        <v>45</v>
-      </c>
-      <c r="J70" s="7">
-        <v>492000</v>
-      </c>
-      <c r="K70" s="7">
-        <v>116850</v>
-      </c>
-    </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B71" t="s">
-        <v>21</v>
-      </c>
-      <c r="C71" t="s">
-        <v>12</v>
-      </c>
-      <c r="D71" t="s">
-        <v>33</v>
-      </c>
-      <c r="J71" s="7">
-        <v>188000</v>
-      </c>
-      <c r="K71" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C72" t="s">
-        <v>42</v>
-      </c>
-      <c r="J72" s="7">
-        <v>188000</v>
-      </c>
-      <c r="K72" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B73" t="s">
-        <v>46</v>
-      </c>
-      <c r="J73" s="7">
-        <v>188000</v>
-      </c>
-      <c r="K73" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B74" t="s">
-        <v>22</v>
-      </c>
-      <c r="C74" t="s">
-        <v>14</v>
-      </c>
-      <c r="D74" t="s">
-        <v>33</v>
-      </c>
-      <c r="J74" s="7">
-        <v>180000</v>
-      </c>
-      <c r="K74" s="7">
-        <v>79380</v>
-      </c>
-    </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C75" t="s">
-        <v>44</v>
-      </c>
-      <c r="J75" s="7">
-        <v>180000</v>
-      </c>
-      <c r="K75" s="7">
-        <v>79380</v>
-      </c>
-    </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B76" t="s">
-        <v>47</v>
-      </c>
-      <c r="J76" s="7">
-        <v>180000</v>
-      </c>
-      <c r="K76" s="7">
-        <v>79380</v>
-      </c>
-    </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B77" t="s">
-        <v>23</v>
-      </c>
-      <c r="C77" t="s">
-        <v>16</v>
-      </c>
-      <c r="D77" t="s">
-        <v>32</v>
-      </c>
-      <c r="J77" s="7">
-        <v>582000</v>
-      </c>
-      <c r="K77" s="7">
-        <v>195231</v>
-      </c>
-    </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C78" t="s">
-        <v>36</v>
-      </c>
-      <c r="J78" s="7">
-        <v>582000</v>
-      </c>
-      <c r="K78" s="7">
-        <v>195231</v>
-      </c>
-    </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B79" t="s">
-        <v>48</v>
-      </c>
-      <c r="J79" s="7">
-        <v>582000</v>
-      </c>
-      <c r="K79" s="7">
-        <v>195231</v>
-      </c>
-    </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B80" t="s">
-        <v>24</v>
-      </c>
-      <c r="C80" t="s">
-        <v>18</v>
-      </c>
-      <c r="D80" t="s">
-        <v>32</v>
-      </c>
-      <c r="J80" s="7">
-        <v>562000</v>
-      </c>
-      <c r="K80" s="7">
-        <v>74746</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C81" t="s">
-        <v>38</v>
-      </c>
-      <c r="J81" s="7">
-        <v>562000</v>
-      </c>
-      <c r="K81" s="7">
-        <v>74746</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B82" t="s">
-        <v>52</v>
-      </c>
-      <c r="J82" s="7">
-        <v>562000</v>
-      </c>
-      <c r="K82" s="7">
-        <v>74746</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>53</v>
-      </c>
-      <c r="J83" s="7">
-        <v>3849000</v>
-      </c>
-      <c r="K83" s="7">
-        <v>1208369</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>26</v>
-      </c>
-      <c r="B84" t="s">
-        <v>11</v>
-      </c>
-      <c r="C84" t="s">
-        <v>12</v>
-      </c>
-      <c r="D84" t="s">
-        <v>33</v>
-      </c>
-      <c r="J84" s="7">
-        <v>293000</v>
-      </c>
-      <c r="K84" s="7">
-        <v>273001</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C85" t="s">
-        <v>42</v>
-      </c>
-      <c r="J85" s="7">
-        <v>293000</v>
-      </c>
-      <c r="K85" s="7">
-        <v>273001</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B86" t="s">
-        <v>37</v>
-      </c>
-      <c r="J86" s="7">
-        <v>293000</v>
-      </c>
-      <c r="K86" s="7">
-        <v>273001</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B87" t="s">
-        <v>25</v>
-      </c>
-      <c r="C87" t="s">
-        <v>20</v>
-      </c>
-      <c r="D87" t="s">
-        <v>33</v>
-      </c>
-      <c r="J87" s="7">
-        <v>68000</v>
-      </c>
-      <c r="K87" s="7">
-        <v>64987</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C88" t="s">
-        <v>40</v>
-      </c>
-      <c r="J88" s="7">
-        <v>68000</v>
-      </c>
-      <c r="K88" s="7">
-        <v>64987</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B89" t="s">
-        <v>51</v>
-      </c>
-      <c r="J89" s="7">
-        <v>68000</v>
-      </c>
-      <c r="K89" s="7">
-        <v>64987</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B90" t="s">
-        <v>13</v>
-      </c>
-      <c r="C90" t="s">
-        <v>14</v>
-      </c>
-      <c r="D90" t="s">
-        <v>32</v>
-      </c>
-      <c r="J90" s="7">
-        <v>224000</v>
-      </c>
-      <c r="K90" s="7">
-        <v>57910</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C91" t="s">
-        <v>44</v>
-      </c>
-      <c r="J91" s="7">
-        <v>224000</v>
-      </c>
-      <c r="K91" s="7">
-        <v>57910</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B92" t="s">
-        <v>39</v>
-      </c>
-      <c r="J92" s="7">
-        <v>224000</v>
-      </c>
-      <c r="K92" s="7">
-        <v>57910</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B93" t="s">
-        <v>15</v>
-      </c>
-      <c r="C93" t="s">
-        <v>16</v>
-      </c>
-      <c r="D93" t="s">
-        <v>32</v>
-      </c>
-      <c r="J93" s="7">
-        <v>978000</v>
-      </c>
-      <c r="K93" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C94" t="s">
-        <v>36</v>
-      </c>
-      <c r="J94" s="7">
-        <v>978000</v>
-      </c>
-      <c r="K94" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B95" t="s">
-        <v>41</v>
-      </c>
-      <c r="J95" s="7">
-        <v>978000</v>
-      </c>
-      <c r="K95" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B96" t="s">
-        <v>17</v>
-      </c>
-      <c r="C96" t="s">
-        <v>18</v>
-      </c>
-      <c r="D96" t="s">
-        <v>33</v>
-      </c>
-      <c r="J96" s="7">
-        <v>932000</v>
-      </c>
-      <c r="K96" s="7">
-        <v>379157</v>
-      </c>
-    </row>
-    <row r="97" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C97" t="s">
-        <v>38</v>
-      </c>
-      <c r="J97" s="7">
-        <v>932000</v>
-      </c>
-      <c r="K97" s="7">
-        <v>379157</v>
-      </c>
-    </row>
-    <row r="98" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B98" t="s">
-        <v>43</v>
-      </c>
-      <c r="J98" s="7">
-        <v>932000</v>
-      </c>
-      <c r="K98" s="7">
-        <v>379157</v>
-      </c>
-    </row>
-    <row r="99" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B99" t="s">
-        <v>19</v>
-      </c>
-      <c r="C99" t="s">
-        <v>20</v>
-      </c>
-      <c r="D99" t="s">
-        <v>33</v>
-      </c>
-      <c r="J99" s="7">
-        <v>854000</v>
-      </c>
-      <c r="K99" s="7">
-        <v>322812</v>
-      </c>
-    </row>
-    <row r="100" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C100" t="s">
-        <v>40</v>
-      </c>
-      <c r="J100" s="7">
-        <v>854000</v>
-      </c>
-      <c r="K100" s="7">
-        <v>322812</v>
-      </c>
-    </row>
-    <row r="101" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B101" t="s">
-        <v>45</v>
-      </c>
-      <c r="J101" s="7">
-        <v>854000</v>
-      </c>
-      <c r="K101" s="7">
-        <v>322812</v>
-      </c>
-    </row>
-    <row r="102" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B102" t="s">
-        <v>21</v>
-      </c>
-      <c r="C102" t="s">
-        <v>12</v>
-      </c>
-      <c r="D102" t="s">
-        <v>33</v>
-      </c>
-      <c r="J102" s="7">
-        <v>81000</v>
-      </c>
-      <c r="K102" s="7">
-        <v>38461</v>
-      </c>
-    </row>
-    <row r="103" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C103" t="s">
-        <v>42</v>
-      </c>
-      <c r="J103" s="7">
-        <v>81000</v>
-      </c>
-      <c r="K103" s="7">
-        <v>38461</v>
-      </c>
-    </row>
-    <row r="104" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B104" t="s">
-        <v>46</v>
-      </c>
-      <c r="J104" s="7">
-        <v>81000</v>
-      </c>
-      <c r="K104" s="7">
-        <v>38461</v>
-      </c>
-    </row>
-    <row r="105" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B105" t="s">
-        <v>22</v>
-      </c>
-      <c r="C105" t="s">
-        <v>14</v>
-      </c>
-      <c r="D105" t="s">
-        <v>32</v>
-      </c>
-      <c r="J105" s="7">
-        <v>169000</v>
-      </c>
-      <c r="K105" s="7">
-        <v>136468</v>
-      </c>
-    </row>
-    <row r="106" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C106" t="s">
-        <v>44</v>
-      </c>
-      <c r="J106" s="7">
-        <v>169000</v>
-      </c>
-      <c r="K106" s="7">
-        <v>136468</v>
-      </c>
-    </row>
-    <row r="107" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B107" t="s">
-        <v>47</v>
-      </c>
-      <c r="J107" s="7">
-        <v>169000</v>
-      </c>
-      <c r="K107" s="7">
-        <v>136468</v>
-      </c>
-    </row>
-    <row r="108" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B108" t="s">
-        <v>23</v>
-      </c>
-      <c r="C108" t="s">
-        <v>16</v>
-      </c>
-      <c r="D108" t="s">
-        <v>32</v>
-      </c>
-      <c r="J108" s="7">
-        <v>61000</v>
-      </c>
-      <c r="K108" s="7">
-        <v>12078</v>
-      </c>
-    </row>
-    <row r="109" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C109" t="s">
-        <v>36</v>
-      </c>
-      <c r="J109" s="7">
-        <v>61000</v>
-      </c>
-      <c r="K109" s="7">
-        <v>12078</v>
-      </c>
-    </row>
-    <row r="110" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B110" t="s">
-        <v>48</v>
-      </c>
-      <c r="J110" s="7">
-        <v>61000</v>
-      </c>
-      <c r="K110" s="7">
-        <v>12078</v>
-      </c>
-    </row>
-    <row r="111" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B111" t="s">
-        <v>24</v>
-      </c>
-      <c r="C111" t="s">
-        <v>18</v>
-      </c>
-      <c r="D111" t="s">
-        <v>32</v>
-      </c>
-      <c r="J111" s="7">
-        <v>645000</v>
-      </c>
-      <c r="K111" s="7">
-        <v>273048</v>
-      </c>
-    </row>
-    <row r="112" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C112" t="s">
-        <v>38</v>
-      </c>
-      <c r="J112" s="7">
-        <v>645000</v>
-      </c>
-      <c r="K112" s="7">
-        <v>273048</v>
-      </c>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B113" t="s">
-        <v>52</v>
-      </c>
-      <c r="J113" s="7">
-        <v>645000</v>
-      </c>
-      <c r="K113" s="7">
-        <v>273048</v>
-      </c>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
-        <v>54</v>
-      </c>
-      <c r="J114" s="7">
-        <v>4305000</v>
-      </c>
-      <c r="K114" s="7">
-        <v>1557922</v>
-      </c>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
-        <v>27</v>
-      </c>
-      <c r="B115" t="s">
-        <v>11</v>
-      </c>
-      <c r="C115" t="s">
-        <v>12</v>
-      </c>
-      <c r="D115" t="s">
-        <v>32</v>
-      </c>
-      <c r="J115" s="7">
-        <v>839000</v>
-      </c>
-      <c r="K115" s="7">
-        <v>406974</v>
-      </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C116" t="s">
-        <v>42</v>
-      </c>
-      <c r="J116" s="7">
-        <v>839000</v>
-      </c>
-      <c r="K116" s="7">
-        <v>406974</v>
-      </c>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B117" t="s">
-        <v>37</v>
-      </c>
-      <c r="J117" s="7">
-        <v>839000</v>
-      </c>
-      <c r="K117" s="7">
-        <v>406974</v>
-      </c>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B118" t="s">
-        <v>13</v>
-      </c>
-      <c r="C118" t="s">
-        <v>14</v>
-      </c>
-      <c r="D118" t="s">
-        <v>33</v>
-      </c>
-      <c r="J118" s="7">
-        <v>729000</v>
-      </c>
-      <c r="K118" s="7">
-        <v>487139</v>
-      </c>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C119" t="s">
-        <v>44</v>
-      </c>
-      <c r="J119" s="7">
-        <v>729000</v>
-      </c>
-      <c r="K119" s="7">
-        <v>487139</v>
-      </c>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B120" t="s">
-        <v>39</v>
-      </c>
-      <c r="J120" s="7">
-        <v>729000</v>
-      </c>
-      <c r="K120" s="7">
-        <v>487139</v>
-      </c>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B121" t="s">
-        <v>15</v>
-      </c>
-      <c r="C121" t="s">
-        <v>16</v>
-      </c>
-      <c r="D121" t="s">
-        <v>32</v>
-      </c>
-      <c r="J121" s="7">
-        <v>826000</v>
-      </c>
-      <c r="K121" s="7">
-        <v>298186</v>
-      </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C122" t="s">
-        <v>36</v>
-      </c>
-      <c r="J122" s="7">
-        <v>826000</v>
-      </c>
-      <c r="K122" s="7">
-        <v>298186</v>
-      </c>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B123" t="s">
-        <v>41</v>
-      </c>
-      <c r="J123" s="7">
-        <v>826000</v>
-      </c>
-      <c r="K123" s="7">
-        <v>298186</v>
-      </c>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B124" t="s">
-        <v>17</v>
-      </c>
-      <c r="C124" t="s">
-        <v>18</v>
-      </c>
-      <c r="D124" t="s">
-        <v>32</v>
-      </c>
-      <c r="J124" s="7">
-        <v>895000</v>
-      </c>
-      <c r="K124" s="7">
-        <v>280583</v>
-      </c>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C125" t="s">
-        <v>38</v>
-      </c>
-      <c r="J125" s="7">
-        <v>895000</v>
-      </c>
-      <c r="K125" s="7">
-        <v>280583</v>
-      </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B126" t="s">
-        <v>43</v>
-      </c>
-      <c r="J126" s="7">
-        <v>895000</v>
-      </c>
-      <c r="K126" s="7">
-        <v>280583</v>
-      </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B127" t="s">
-        <v>19</v>
-      </c>
-      <c r="C127" t="s">
-        <v>20</v>
-      </c>
-      <c r="D127" t="s">
-        <v>32</v>
-      </c>
-      <c r="J127" s="7">
-        <v>341000</v>
-      </c>
-      <c r="K127" s="7">
-        <v>129785</v>
-      </c>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C128" t="s">
-        <v>40</v>
-      </c>
-      <c r="J128" s="7">
-        <v>341000</v>
-      </c>
-      <c r="K128" s="7">
-        <v>129785</v>
-      </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B129" t="s">
-        <v>45</v>
-      </c>
-      <c r="J129" s="7">
-        <v>341000</v>
-      </c>
-      <c r="K129" s="7">
-        <v>129785</v>
-      </c>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
-        <v>55</v>
-      </c>
-      <c r="J130" s="7">
-        <v>3630000</v>
-      </c>
-      <c r="K130" s="7">
-        <v>1602667</v>
-      </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
-        <v>31</v>
-      </c>
-      <c r="J131" s="7">
-        <v>19695000</v>
-      </c>
-      <c r="K131" s="7">
         <v>8340291</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed money no. format
</commit_message>
<xml_diff>
--- a/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
+++ b/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Managing Multiple Project Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05804C0A-BB80-B549-807A-EB16114D82CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F56A3CF-93A6-DE44-8670-5D4643DA7643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12880" yWindow="760" windowWidth="17360" windowHeight="17420" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="3" r:id="rId1"/>
@@ -201,7 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -215,13 +215,33 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="15">
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
     <dxf>
       <alignment horizontal="right"/>
     </dxf>
@@ -1467,11 +1487,11 @@
     </i>
   </colItems>
   <dataFields count="2">
-    <dataField name="Budget " fld="8" baseField="0" baseItem="0"/>
-    <dataField name="Actual " fld="9" baseField="0" baseItem="0"/>
+    <dataField name="Budget " fld="8" baseField="0" baseItem="0" numFmtId="3"/>
+    <dataField name="Actual " fld="9" baseField="0" baseItem="0" numFmtId="3"/>
   </dataFields>
-  <formats count="2">
-    <format dxfId="1">
+  <formats count="4">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -1480,8 +1500,26 @@
         </references>
       </pivotArea>
     </format>
+    <format dxfId="7">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
     <format dxfId="0">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+      <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
             <x v="1"/>
@@ -1509,17 +1547,17 @@
     <tableColumn id="1" xr3:uid="{73B096BE-E208-2142-8042-C8FF7EBE9CB4}" name="Project"/>
     <tableColumn id="2" xr3:uid="{9FEE26CA-FD34-8940-B511-23005FD52FD9}" name="Task"/>
     <tableColumn id="3" xr3:uid="{13477DA8-3E2B-9140-828B-5E4EEC4B192E}" name="Manager"/>
-    <tableColumn id="4" xr3:uid="{6F6235F3-DCA0-BE4A-80AD-F124C1F29DF7}" name="Start Date" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{6F6235F3-DCA0-BE4A-80AD-F124C1F29DF7}" name="Start Date" dataDxfId="14"/>
     <tableColumn id="5" xr3:uid="{906D9425-A9AF-D946-BD7E-AABF37A5C06F}" name="Duration"/>
-    <tableColumn id="9" xr3:uid="{49251E86-4677-9C41-8F83-14B60BE792A2}" name="End Date" dataDxfId="2">
+    <tableColumn id="9" xr3:uid="{49251E86-4677-9C41-8F83-14B60BE792A2}" name="End Date" dataDxfId="9">
       <calculatedColumnFormula>WORKDAY.INTL(Project_Data[[#This Row],[Start Date]]-1,Project_Data[[#This Row],[Duration]],7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5410ED6D-ABC2-B749-B761-98A3ACF6E8B5}" name="Days completed" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{1E1A1903-5E63-2C42-A785-7622E4CE1FFD}" name="Progress" dataDxfId="5">
+    <tableColumn id="10" xr3:uid="{5410ED6D-ABC2-B749-B761-98A3ACF6E8B5}" name="Days completed" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{1E1A1903-5E63-2C42-A785-7622E4CE1FFD}" name="Progress" dataDxfId="12">
       <calculatedColumnFormula>Project_Data[[#This Row],[Days completed]]/Project_Data[[#This Row],[Duration]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5529251C-746B-0F49-8B21-221411C8E693}" name="Budget" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{2781FA1C-8107-3A45-8365-873CEB86F752}" name="Actual" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{5529251C-746B-0F49-8B21-221411C8E693}" name="Budget" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{2781FA1C-8107-3A45-8365-873CEB86F752}" name="Actual" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1825,7 +1863,7 @@
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1900,10 +1938,10 @@
       <c r="H6" s="5">
         <v>0.375</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="3">
         <v>96000</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="3">
         <v>32256</v>
       </c>
     </row>
@@ -1929,10 +1967,10 @@
       <c r="H7" s="5">
         <v>0.44444444444444442</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="3">
         <v>513000</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="3">
         <v>226233</v>
       </c>
     </row>
@@ -1958,10 +1996,10 @@
       <c r="H8" s="5">
         <v>0.6</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="3">
         <v>616000</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="3">
         <v>401579</v>
       </c>
     </row>
@@ -1987,10 +2025,10 @@
       <c r="H9" s="5">
         <v>1</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="3">
         <v>817000</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="3">
         <v>807069</v>
       </c>
     </row>
@@ -2016,10 +2054,10 @@
       <c r="H10" s="5">
         <v>0.42857142857142855</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="3">
         <v>372000</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="3">
         <v>173166</v>
       </c>
     </row>
@@ -2045,10 +2083,10 @@
       <c r="H11" s="5">
         <v>0.2</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="3">
         <v>50000</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="3">
         <v>8400</v>
       </c>
     </row>
@@ -2074,10 +2112,10 @@
       <c r="H12" s="5">
         <v>0.3</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="3">
         <v>807000</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="3">
         <v>262679</v>
       </c>
     </row>
@@ -2103,10 +2141,10 @@
       <c r="H13" s="5">
         <v>0</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="3">
         <v>691000</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="3">
         <v>0</v>
       </c>
     </row>
@@ -2135,10 +2173,10 @@
       <c r="H14" s="5">
         <v>0.88888888888888884</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="3">
         <v>787000</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="3">
         <v>727188</v>
       </c>
     </row>
@@ -2164,10 +2202,10 @@
       <c r="H15" s="5">
         <v>0.2</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="3">
         <v>228000</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="3">
         <v>47880</v>
       </c>
     </row>
@@ -2193,10 +2231,10 @@
       <c r="H16" s="5">
         <v>0</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I16" s="3">
         <v>147000</v>
       </c>
-      <c r="J16" s="9">
+      <c r="J16" s="3">
         <v>0</v>
       </c>
     </row>
@@ -2222,10 +2260,10 @@
       <c r="H17" s="5">
         <v>0.625</v>
       </c>
-      <c r="I17" s="9">
+      <c r="I17" s="3">
         <v>338000</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17" s="3">
         <v>205123</v>
       </c>
     </row>
@@ -2251,10 +2289,10 @@
       <c r="H18" s="5">
         <v>0.3</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18" s="3">
         <v>857000</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="3">
         <v>305949</v>
       </c>
     </row>
@@ -2280,10 +2318,10 @@
       <c r="H19" s="5">
         <v>0.5</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I19" s="3">
         <v>602000</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19" s="3">
         <v>322371</v>
       </c>
     </row>
@@ -2309,10 +2347,10 @@
       <c r="H20" s="5">
         <v>0.5</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="3">
         <v>990000</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J20" s="3">
         <v>451440</v>
       </c>
     </row>
@@ -2341,10 +2379,10 @@
       <c r="H21" s="5">
         <v>0.4</v>
       </c>
-      <c r="I21" s="9">
+      <c r="I21" s="3">
         <v>218000</v>
       </c>
-      <c r="J21" s="9">
+      <c r="J21" s="3">
         <v>97337</v>
       </c>
     </row>
@@ -2370,10 +2408,10 @@
       <c r="H22" s="5">
         <v>0.5</v>
       </c>
-      <c r="I22" s="9">
+      <c r="I22" s="3">
         <v>416000</v>
       </c>
-      <c r="J22" s="9">
+      <c r="J22" s="3">
         <v>175015</v>
       </c>
     </row>
@@ -2399,10 +2437,10 @@
       <c r="H23" s="5">
         <v>0.5</v>
       </c>
-      <c r="I23" s="9">
+      <c r="I23" s="3">
         <v>393000</v>
       </c>
-      <c r="J23" s="9">
+      <c r="J23" s="3">
         <v>177440</v>
       </c>
     </row>
@@ -2428,10 +2466,10 @@
       <c r="H24" s="5">
         <v>0.4</v>
       </c>
-      <c r="I24" s="9">
+      <c r="I24" s="3">
         <v>86000</v>
       </c>
-      <c r="J24" s="9">
+      <c r="J24" s="3">
         <v>31046</v>
       </c>
     </row>
@@ -2457,10 +2495,10 @@
       <c r="H25" s="5">
         <v>0.33333333333333331</v>
       </c>
-      <c r="I25" s="9">
+      <c r="I25" s="3">
         <v>732000</v>
       </c>
-      <c r="J25" s="9">
+      <c r="J25" s="3">
         <v>261324</v>
       </c>
     </row>
@@ -2486,10 +2524,10 @@
       <c r="H26" s="5">
         <v>0.25</v>
       </c>
-      <c r="I26" s="9">
+      <c r="I26" s="3">
         <v>492000</v>
       </c>
-      <c r="J26" s="9">
+      <c r="J26" s="3">
         <v>116850</v>
       </c>
     </row>
@@ -2515,10 +2553,10 @@
       <c r="H27" s="5">
         <v>0</v>
       </c>
-      <c r="I27" s="9">
+      <c r="I27" s="3">
         <v>188000</v>
       </c>
-      <c r="J27" s="9">
+      <c r="J27" s="3">
         <v>0</v>
       </c>
     </row>
@@ -2544,10 +2582,10 @@
       <c r="H28" s="5">
         <v>0.42857142857142855</v>
       </c>
-      <c r="I28" s="9">
+      <c r="I28" s="3">
         <v>180000</v>
       </c>
-      <c r="J28" s="9">
+      <c r="J28" s="3">
         <v>79380</v>
       </c>
     </row>
@@ -2573,10 +2611,10 @@
       <c r="H29" s="5">
         <v>0.4</v>
       </c>
-      <c r="I29" s="9">
+      <c r="I29" s="3">
         <v>582000</v>
       </c>
-      <c r="J29" s="9">
+      <c r="J29" s="3">
         <v>195231</v>
       </c>
     </row>
@@ -2602,10 +2640,10 @@
       <c r="H30" s="5">
         <v>0.1111111111111111</v>
       </c>
-      <c r="I30" s="9">
+      <c r="I30" s="3">
         <v>562000</v>
       </c>
-      <c r="J30" s="9">
+      <c r="J30" s="3">
         <v>74746</v>
       </c>
     </row>
@@ -2634,10 +2672,10 @@
       <c r="H31" s="5">
         <v>1</v>
       </c>
-      <c r="I31" s="9">
+      <c r="I31" s="3">
         <v>293000</v>
       </c>
-      <c r="J31" s="9">
+      <c r="J31" s="3">
         <v>273001</v>
       </c>
     </row>
@@ -2663,10 +2701,10 @@
       <c r="H32" s="5">
         <v>1</v>
       </c>
-      <c r="I32" s="9">
+      <c r="I32" s="3">
         <v>68000</v>
       </c>
-      <c r="J32" s="9">
+      <c r="J32" s="3">
         <v>64987</v>
       </c>
     </row>
@@ -2692,10 +2730,10 @@
       <c r="H33" s="5">
         <v>0.44444444444444442</v>
       </c>
-      <c r="I33" s="9">
+      <c r="I33" s="3">
         <v>224000</v>
       </c>
-      <c r="J33" s="9">
+      <c r="J33" s="3">
         <v>57910</v>
       </c>
     </row>
@@ -2721,10 +2759,10 @@
       <c r="H34" s="5">
         <v>0</v>
       </c>
-      <c r="I34" s="9">
+      <c r="I34" s="3">
         <v>978000</v>
       </c>
-      <c r="J34" s="9">
+      <c r="J34" s="3">
         <v>0</v>
       </c>
     </row>
@@ -2750,10 +2788,10 @@
       <c r="H35" s="5">
         <v>0.42857142857142855</v>
       </c>
-      <c r="I35" s="9">
+      <c r="I35" s="3">
         <v>932000</v>
       </c>
-      <c r="J35" s="9">
+      <c r="J35" s="3">
         <v>379157</v>
       </c>
     </row>
@@ -2779,10 +2817,10 @@
       <c r="H36" s="5">
         <v>0.25</v>
       </c>
-      <c r="I36" s="9">
+      <c r="I36" s="3">
         <v>854000</v>
       </c>
-      <c r="J36" s="9">
+      <c r="J36" s="3">
         <v>322812</v>
       </c>
     </row>
@@ -2808,10 +2846,10 @@
       <c r="H37" s="5">
         <v>0.5</v>
       </c>
-      <c r="I37" s="9">
+      <c r="I37" s="3">
         <v>81000</v>
       </c>
-      <c r="J37" s="9">
+      <c r="J37" s="3">
         <v>38461</v>
       </c>
     </row>
@@ -2837,10 +2875,10 @@
       <c r="H38" s="5">
         <v>0.83333333333333337</v>
       </c>
-      <c r="I38" s="9">
+      <c r="I38" s="3">
         <v>169000</v>
       </c>
-      <c r="J38" s="9">
+      <c r="J38" s="3">
         <v>136468</v>
       </c>
     </row>
@@ -2866,10 +2904,10 @@
       <c r="H39" s="5">
         <v>0.25</v>
       </c>
-      <c r="I39" s="9">
+      <c r="I39" s="3">
         <v>61000</v>
       </c>
-      <c r="J39" s="9">
+      <c r="J39" s="3">
         <v>12078</v>
       </c>
     </row>
@@ -2895,10 +2933,10 @@
       <c r="H40" s="5">
         <v>0.42857142857142855</v>
       </c>
-      <c r="I40" s="9">
+      <c r="I40" s="3">
         <v>645000</v>
       </c>
-      <c r="J40" s="9">
+      <c r="J40" s="3">
         <v>273048</v>
       </c>
     </row>
@@ -2927,10 +2965,10 @@
       <c r="H41" s="5">
         <v>0.5</v>
       </c>
-      <c r="I41" s="9">
+      <c r="I41" s="3">
         <v>839000</v>
       </c>
-      <c r="J41" s="9">
+      <c r="J41" s="3">
         <v>406974</v>
       </c>
     </row>
@@ -2956,10 +2994,10 @@
       <c r="H42" s="5">
         <v>0.8</v>
       </c>
-      <c r="I42" s="9">
+      <c r="I42" s="3">
         <v>729000</v>
       </c>
-      <c r="J42" s="9">
+      <c r="J42" s="3">
         <v>487139</v>
       </c>
     </row>
@@ -2985,10 +3023,10 @@
       <c r="H43" s="5">
         <v>0.42857142857142855</v>
       </c>
-      <c r="I43" s="9">
+      <c r="I43" s="3">
         <v>826000</v>
       </c>
-      <c r="J43" s="9">
+      <c r="J43" s="3">
         <v>298186</v>
       </c>
     </row>
@@ -3014,10 +3052,10 @@
       <c r="H44" s="5">
         <v>0.2857142857142857</v>
       </c>
-      <c r="I44" s="9">
+      <c r="I44" s="3">
         <v>895000</v>
       </c>
-      <c r="J44" s="9">
+      <c r="J44" s="3">
         <v>280583</v>
       </c>
     </row>
@@ -3043,10 +3081,10 @@
       <c r="H45" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="I45" s="9">
+      <c r="I45" s="3">
         <v>341000</v>
       </c>
-      <c r="J45" s="9">
+      <c r="J45" s="3">
         <v>129785</v>
       </c>
     </row>
@@ -3054,10 +3092,10 @@
       <c r="A46" t="s">
         <v>33</v>
       </c>
-      <c r="I46" s="9">
+      <c r="I46" s="3">
         <v>19695000</v>
       </c>
-      <c r="J46" s="9">
+      <c r="J46" s="3">
         <v>8340291</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Inserted progress bar chart
</commit_message>
<xml_diff>
--- a/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
+++ b/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Managing Multiple Project Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A607F2CC-5FA5-A747-8053-46802B5C81CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF3EB1D-0060-5843-83DE-B4DB3D529D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12880" yWindow="760" windowWidth="17360" windowHeight="17420" activeTab="1" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" activeTab="1" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="3" r:id="rId1"/>
@@ -204,20 +204,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -240,7 +231,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -320,6 +311,1113 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU" sz="1200">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>OVERALL TASK PROGRESS</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="1.7230972084835771E-2"/>
+          <c:y val="9.2854047396391665E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-BD"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Workings!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Not Started</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="0;\-0;" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-BD"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Workings!$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4915-7E41-9B8B-FDBCFE6E6C0F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Workings!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>In Progress</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-BD"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Workings!$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4915-7E41-9B8B-FDBCFE6E6C0F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Workings!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Completed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="0;\-0;" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-BD"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Workings!$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4915-7E41-9B8B-FDBCFE6E6C0F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="0"/>
+        <c:overlap val="100"/>
+        <c:axId val="1614655279"/>
+        <c:axId val="1903939599"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1614655279"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1903939599"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1903939599"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1614655279"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0"/>
+          <c:y val="0.33184683043888474"/>
+          <c:w val="0.73805683450224535"/>
+          <c:h val="0.22613235528421916"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-BD"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-BD"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>443566</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>186764</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Chart 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA32CE28-BBA5-2544-8D6D-0BDA18B37B6A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -333,8 +1431,8 @@
       <sheetName val="Dashboard Protection"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2">
         <row r="2">
           <cell r="E2" t="str">
@@ -374,9 +1472,9 @@
         </row>
       </sheetData>
       <sheetData sheetId="3"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3135,10 +4233,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F58449-19E8-9241-BC9F-FCB0CCBB3CD8}">
-  <dimension ref="A3:B7"/>
+  <dimension ref="B2:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3146,53 +4244,51 @@
     <col min="1" max="1" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
         <v>34</v>
       </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3">
         <f>COUNTIF(Dashboard!H6:H50, "="&amp;0)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4">
+      <c r="C3">
         <f>COUNTIFS(Dashboard!H6:H50, "&lt;&gt;"&amp;0,Dashboard!H6:H50, "&lt;"&amp;1)</f>
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5">
+      <c r="D3">
         <f>COUNTIF(Dashboard!H6:H50, "="&amp;1)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="E3">
+        <f>SUM(B3:C3)</f>
         <v>37</v>
       </c>
-      <c r="B6">
-        <f>SUM(B3:B4)</f>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="9">
-        <f>SUM(B5:B6)</f>
+      <c r="F3">
+        <f>SUM(D3:E3)</f>
         <v>40</v>
       </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Calculated days completed and remaining
</commit_message>
<xml_diff>
--- a/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
+++ b/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Managing Multiple Project Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE20D53-AA61-1C44-8F1D-EC4C6571964D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291F19BB-5BF4-7F48-8FBA-E092A64920BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7240" yWindow="760" windowWidth="23000" windowHeight="17420" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
+    <workbookView xWindow="13520" yWindow="760" windowWidth="16720" windowHeight="17420" activeTab="1" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </externalReferences>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="12" r:id="rId5"/>
+    <pivotCache cacheId="14" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="44">
   <si>
     <t>Project</t>
   </si>
@@ -147,6 +147,9 @@
     <t>Grand Total</t>
   </si>
   <si>
+    <t>Sum of Duration</t>
+  </si>
+  <si>
     <t>Not Started</t>
   </si>
   <si>
@@ -160,6 +163,18 @@
   </si>
   <si>
     <t>Total Tasks</t>
+  </si>
+  <si>
+    <t>Sum of Days completed</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Days Completed</t>
+  </si>
+  <si>
+    <t>Days Remaining</t>
   </si>
 </sst>
 </file>
@@ -217,7 +232,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -230,6 +245,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
@@ -2085,7 +2104,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{49A324D7-DAC3-AE4C-8B42-860D7EF2D1B0}" name="PivotTable2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{49A324D7-DAC3-AE4C-8B42-860D7EF2D1B0}" name="PivotTable2" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A9:J50" firstHeaderRow="0" firstDataRow="1" firstDataCol="8"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -2649,6 +2668,51 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8BFD054C-FC60-7949-A08A-A713A0535ED3}" name="PivotTable3" cacheId="14" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="I2:J4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField dataField="1" numFmtId="3" showAll="0"/>
+    <pivotField numFmtId="9" showAll="0"/>
+    <pivotField numFmtId="3" showAll="0"/>
+    <pivotField numFmtId="3" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Days completed" fld="6" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Duration" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D0736C60-3115-3B4B-9BB9-B8998762F286}" name="Project_Data" displayName="Project_Data" ref="A1:J41" totalsRowShown="0">
   <autoFilter ref="A1:J41" xr:uid="{D0736C60-3115-3B4B-9BB9-B8998762F286}"/>
@@ -2971,8 +3035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18BA6329-E680-5548-BB82-D6FB67EB7003}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4219,35 +4283,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F58449-19E8-9241-BC9F-FCB0CCBB3CD8}">
-  <dimension ref="B2:F6"/>
+  <dimension ref="B2:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B3">
         <f>COUNTIF(Dashboard!H10:H54, "="&amp;0)</f>
         <v>4</v>
@@ -4268,9 +4338,37 @@
         <f>SUM(D3:E3)</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="9"/>
+      <c r="I3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="9">
+        <v>112</v>
+      </c>
+      <c r="L3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="4">
+        <f>GETPIVOTDATA("Sum of Days completed",$I$2)/GETPIVOTDATA("Sum of Duration",$I$2)</f>
+        <v>0.42105263157894735</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="I4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="9">
+        <v>266</v>
+      </c>
+      <c r="L4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4" s="4">
+        <f>1-M3</f>
+        <v>0.57894736842105265</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B6" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added actual and budget pivot
</commit_message>
<xml_diff>
--- a/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
+++ b/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Managing Multiple Project Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3EDDA67-E3E7-E248-A17E-80D53A3F3B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBCEAED-F3D4-E94B-9135-173355EAEE72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6840" yWindow="760" windowWidth="23400" windowHeight="17420" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
+    <workbookView xWindow="6900" yWindow="760" windowWidth="23400" windowHeight="17420" activeTab="1" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </externalReferences>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId5"/>
+    <pivotCache cacheId="15" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="44">
   <si>
     <t>Project</t>
   </si>
@@ -181,8 +181,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="168" formatCode="0.0,,\M;\-0.0,,\M"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -232,7 +233,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -251,6 +252,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2997,7 +2999,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{49A324D7-DAC3-AE4C-8B42-860D7EF2D1B0}" name="PivotTable2" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{49A324D7-DAC3-AE4C-8B42-860D7EF2D1B0}" name="PivotTable2" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A10:J51" firstHeaderRow="0" firstDataRow="1" firstDataCol="8"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -3562,7 +3564,52 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8BFD054C-FC60-7949-A08A-A713A0535ED3}" name="PivotTable3" cacheId="14" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{73EC0C1C-71D5-2447-BF2E-80B6A5A74F04}" name="PivotTable4" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="P3:Q4" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="10">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField numFmtId="3" showAll="0"/>
+    <pivotField numFmtId="9" showAll="0"/>
+    <pivotField dataField="1" numFmtId="3" showAll="0"/>
+    <pivotField dataField="1" numFmtId="3" showAll="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Actual " fld="9" baseField="0" baseItem="0" numFmtId="168"/>
+    <dataField name="Budget " fld="8" baseField="0" baseItem="0" numFmtId="168"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8BFD054C-FC60-7949-A08A-A713A0535ED3}" name="PivotTable3" cacheId="15" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="I2:J4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -3928,7 +3975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18BA6329-E680-5548-BB82-D6FB67EB7003}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
@@ -5176,10 +5223,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F58449-19E8-9241-BC9F-FCB0CCBB3CD8}">
-  <dimension ref="B2:M6"/>
+  <dimension ref="B2:Q6"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5188,9 +5235,11 @@
     <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.6640625" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>35</v>
       </c>
@@ -5210,7 +5259,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B3">
         <f>COUNTIF(Dashboard!H11:H55, "="&amp;0)</f>
         <v>4</v>
@@ -5244,8 +5293,14 @@
         <f>GETPIVOTDATA("Sum of Days completed",$I$2)/GETPIVOTDATA("Sum of Duration",$I$2)</f>
         <v>0.42105263157894735</v>
       </c>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="P3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="I4" s="10" t="s">
         <v>34</v>
       </c>
@@ -5259,8 +5314,14 @@
         <f>1-M3</f>
         <v>0.57894736842105265</v>
       </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="P4" s="12">
+        <v>8340291</v>
+      </c>
+      <c r="Q4" s="12">
+        <v>19695000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B6" s="11"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added budget vs actual chart
</commit_message>
<xml_diff>
--- a/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
+++ b/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Managing Multiple Project Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787AAEE0-5716-1545-9267-811CC57FF93F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5F9D9E-0E11-4949-B16F-C4C130023279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
   </bookViews>
@@ -1285,6 +1285,1136 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Multiple Project Progress Management.xlsx]Workings!PivotTable4</c:name>
+    <c:fmtId val="3"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="Britannic Bold" panose="020B0903060703020204" pitchFamily="34" charset="77"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1600">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="Britannic Bold" panose="020B0903060703020204" pitchFamily="34" charset="77"/>
+              </a:rPr>
+              <a:t>BUDGET VS ACTUAL</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.8509264037555559E-2"/>
+          <c:y val="6.6204944891271975E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Britannic Bold" panose="020B0903060703020204" pitchFamily="34" charset="77"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-BD"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-BD"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:separator>
+</c:separator>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="FF8A84"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-BD"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:separator>
+</c:separator>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="FF8A84"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-BD"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="1"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:separator>
+</c:separator>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-BD"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="1"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:separator>
+</c:separator>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-BD"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:separator>
+</c:separator>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-BD"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="1"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:separator>
+</c:separator>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="FF8A84"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-BD"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:separator>
+</c:separator>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="FF8A84"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-BD"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="1"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:separator>
+</c:separator>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-BD"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:separator>
+</c:separator>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-BD"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="1"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:separator>
+</c:separator>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="FF8A84"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-BD"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:separator>
+</c:separator>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="FF8A84"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-BD"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="1"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:separator>
+</c:separator>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.6511627906976744E-2"/>
+          <c:y val="0.37987836886242876"/>
+          <c:w val="0.90697674418604646"/>
+          <c:h val="0.55508098073106704"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Workings!$Q$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-5C72-4D46-9888-220B9196E5EF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-BD"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:separator>
+</c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Workings!$Q$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Workings!$Q$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.0,,\M;\-0.0,,\M</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8340291</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5C72-4D46-9888-220B9196E5EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Workings!$R$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Budget </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF8A84"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-5C72-4D46-9888-220B9196E5EF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-BD"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:separator>
+</c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Workings!$Q$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Workings!$R$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.0,,\M;\-0.0,,\M</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>19695000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5C72-4D46-9888-220B9196E5EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="0"/>
+        <c:overlap val="-30"/>
+        <c:axId val="2042557552"/>
+        <c:axId val="2042265504"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2042557552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2042265504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2042265504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.0,,\M;\-0.0,,\M" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2042557552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-BD"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1405,6 +2535,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -2606,6 +3776,511 @@
       <cs:styleClr val="auto"/>
     </cs:lnRef>
     <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -3064,6 +4739,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4EEADD4-20BF-DC41-9A30-F226C92EEBA1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3135,12 +4848,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.3805</cdr:x>
-      <cdr:y>0.48522</cdr:y>
+      <cdr:x>0.37405</cdr:x>
+      <cdr:y>0.49221</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.76273</cdr:x>
-      <cdr:y>0.8257</cdr:y>
+      <cdr:x>0.75628</cdr:x>
+      <cdr:y>0.83269</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="Workings!$Q$5">
       <cdr:nvSpPr>
@@ -3155,7 +4868,7 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="749011" y="881199"/>
+          <a:off x="736311" y="893899"/>
           <a:ext cx="752420" cy="618346"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
@@ -4442,7 +6155,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{73EC0C1C-71D5-2447-BF2E-80B6A5A74F04}" name="PivotTable4" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{73EC0C1C-71D5-2447-BF2E-80B6A5A74F04}" name="PivotTable4" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="Q3:R4" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -4474,6 +6187,134 @@
     <dataField name="Actual " fld="9" baseField="0" baseItem="0" numFmtId="168"/>
     <dataField name="Budget " fld="8" baseField="0" baseItem="0" numFmtId="168"/>
   </dataFields>
+  <chartFormats count="14">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -4854,7 +6695,7 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6103,8 +7944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F58449-19E8-9241-BC9F-FCB0CCBB3CD8}">
   <dimension ref="B2:R6"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added project and manager slicers
</commit_message>
<xml_diff>
--- a/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
+++ b/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Managing Multiple Project Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5F9D9E-0E11-4949-B16F-C4C130023279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4861F09-A61C-A849-8BA7-69E376771CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
+    <workbookView xWindow="5100" yWindow="760" windowWidth="25140" windowHeight="17420" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="3" r:id="rId1"/>
@@ -20,11 +20,24 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
+  <definedNames>
+    <definedName name="Slicer_Manager">#N/A</definedName>
+    <definedName name="Slicer_Project">#N/A</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
     <pivotCache cacheId="15" r:id="rId5"/>
   </pivotCaches>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
+      <x14:slicerCaches>
+        <x14:slicerCache r:id="rId6"/>
+        <x14:slicerCache r:id="rId7"/>
+      </x14:slicerCaches>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -264,7 +277,19 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="14">
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
@@ -4777,6 +4802,162 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="6" name="Project">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C593B1BF-D3B4-ED98-12DA-D07A1DCDC08C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Project"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="76200" y="812800"/>
+              <a:ext cx="3479800" cy="774700"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>472350</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="7" name="Manager">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43D25168-AF9F-78D9-BD0F-C1A005DD71A5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Manager"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3733800" y="812800"/>
+              <a:ext cx="3761650" cy="774700"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5098,7 +5279,7 @@
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
+      <x14:pivotCacheDefinition pivotCacheId="1718326313"/>
     </ext>
   </extLst>
 </pivotCacheDefinition>
@@ -6105,7 +6286,7 @@
     <dataField name="Actual " fld="9" baseField="0" baseItem="0" numFmtId="3"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="3">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6114,7 +6295,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6123,7 +6304,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="5">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6132,7 +6313,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="4">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6372,6 +6553,51 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Project" xr10:uid="{9EF967C5-BC98-5340-BB32-BFAC0DF0F8C4}" sourceName="Project">
+  <pivotTables>
+    <pivotTable tabId="3" name="PivotTable2"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="1718326313">
+      <items count="5">
+        <i x="4" s="1"/>
+        <i x="3" s="1"/>
+        <i x="0" s="1"/>
+        <i x="1" s="1"/>
+        <i x="2" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache2.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Manager" xr10:uid="{978C6F23-8125-2640-A99C-52F8BB22D398}" sourceName="Manager">
+  <pivotTables>
+    <pivotTable tabId="3" name="PivotTable2"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="1718326313">
+      <items count="5">
+        <i x="0" s="1"/>
+        <i x="4" s="1"/>
+        <i x="2" s="1"/>
+        <i x="1" s="1"/>
+        <i x="3" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Project" xr10:uid="{40278B86-7F81-3B47-A35F-6B59D57646AB}" cache="Slicer_Project" caption="Project" columnCount="5" rowHeight="255600"/>
+  <slicer name="Manager" xr10:uid="{90F1F47E-BEF9-4B4F-9E49-C7D1AE3FCB94}" cache="Slicer_Manager" caption="Manager" columnCount="5" rowHeight="251883"/>
+</slicers>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D0736C60-3115-3B4B-9BB9-B8998762F286}" name="Project_Data" displayName="Project_Data" ref="A1:J41" totalsRowShown="0">
   <autoFilter ref="A1:J41" xr:uid="{D0736C60-3115-3B4B-9BB9-B8998762F286}"/>
@@ -6379,17 +6605,17 @@
     <tableColumn id="1" xr3:uid="{73B096BE-E208-2142-8042-C8FF7EBE9CB4}" name="Project"/>
     <tableColumn id="2" xr3:uid="{9FEE26CA-FD34-8940-B511-23005FD52FD9}" name="Task"/>
     <tableColumn id="3" xr3:uid="{13477DA8-3E2B-9140-828B-5E4EEC4B192E}" name="Manager"/>
-    <tableColumn id="4" xr3:uid="{6F6235F3-DCA0-BE4A-80AD-F124C1F29DF7}" name="Start Date" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{6F6235F3-DCA0-BE4A-80AD-F124C1F29DF7}" name="Start Date" dataDxfId="13"/>
     <tableColumn id="5" xr3:uid="{906D9425-A9AF-D946-BD7E-AABF37A5C06F}" name="Duration"/>
-    <tableColumn id="9" xr3:uid="{49251E86-4677-9C41-8F83-14B60BE792A2}" name="End Date" dataDxfId="4">
+    <tableColumn id="9" xr3:uid="{49251E86-4677-9C41-8F83-14B60BE792A2}" name="End Date" dataDxfId="8">
       <calculatedColumnFormula>WORKDAY.INTL(Project_Data[[#This Row],[Start Date]]-1,Project_Data[[#This Row],[Duration]],7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5410ED6D-ABC2-B749-B761-98A3ACF6E8B5}" name="Days completed" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{1E1A1903-5E63-2C42-A785-7622E4CE1FFD}" name="Progress" dataDxfId="7">
+    <tableColumn id="10" xr3:uid="{5410ED6D-ABC2-B749-B761-98A3ACF6E8B5}" name="Days completed" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{1E1A1903-5E63-2C42-A785-7622E4CE1FFD}" name="Progress" dataDxfId="11">
       <calculatedColumnFormula>Project_Data[[#This Row],[Days completed]]/Project_Data[[#This Row],[Duration]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5529251C-746B-0F49-8B21-221411C8E693}" name="Budget" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{2781FA1C-8107-3A45-8365-873CEB86F752}" name="Actual" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{5529251C-746B-0F49-8B21-221411C8E693}" name="Budget" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{2781FA1C-8107-3A45-8365-873CEB86F752}" name="Actual" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6695,7 +6921,7 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7937,6 +8163,13 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId3"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed progress chart no. format
</commit_message>
<xml_diff>
--- a/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
+++ b/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Managing Multiple Project Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A17518-B785-DF43-9A54-9850DAC85D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BED600-9988-5F4A-9082-804571F4BAC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5100" yWindow="760" windowWidth="25140" windowHeight="17420" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
   </bookViews>
@@ -277,7 +277,43 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="34">
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="right"/>
     </dxf>
@@ -615,6 +651,7 @@
             </c:extLst>
           </c:dPt>
           <c:dLbls>
+            <c:numFmt formatCode="0;\-0;" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -6310,7 +6347,7 @@
     <dataField name="Actual " fld="9" baseField="0" baseItem="0" numFmtId="3"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="15">
+    <format dxfId="27">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6319,7 +6356,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="26">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6328,7 +6365,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="25">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6337,7 +6374,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="24">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6669,17 +6706,17 @@
     <tableColumn id="1" xr3:uid="{73B096BE-E208-2142-8042-C8FF7EBE9CB4}" name="Project"/>
     <tableColumn id="2" xr3:uid="{9FEE26CA-FD34-8940-B511-23005FD52FD9}" name="Task"/>
     <tableColumn id="3" xr3:uid="{13477DA8-3E2B-9140-828B-5E4EEC4B192E}" name="Manager"/>
-    <tableColumn id="4" xr3:uid="{6F6235F3-DCA0-BE4A-80AD-F124C1F29DF7}" name="Start Date" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{6F6235F3-DCA0-BE4A-80AD-F124C1F29DF7}" name="Start Date" dataDxfId="33"/>
     <tableColumn id="5" xr3:uid="{906D9425-A9AF-D946-BD7E-AABF37A5C06F}" name="Duration"/>
-    <tableColumn id="9" xr3:uid="{49251E86-4677-9C41-8F83-14B60BE792A2}" name="End Date" dataDxfId="16">
+    <tableColumn id="9" xr3:uid="{49251E86-4677-9C41-8F83-14B60BE792A2}" name="End Date" dataDxfId="28">
       <calculatedColumnFormula>WORKDAY.INTL(Project_Data[[#This Row],[Start Date]]-1,Project_Data[[#This Row],[Duration]],7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5410ED6D-ABC2-B749-B761-98A3ACF6E8B5}" name="Days completed" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{1E1A1903-5E63-2C42-A785-7622E4CE1FFD}" name="Progress" dataDxfId="19">
+    <tableColumn id="10" xr3:uid="{5410ED6D-ABC2-B749-B761-98A3ACF6E8B5}" name="Days completed" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{1E1A1903-5E63-2C42-A785-7622E4CE1FFD}" name="Progress" dataDxfId="31">
       <calculatedColumnFormula>Project_Data[[#This Row],[Days completed]]/Project_Data[[#This Row],[Duration]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5529251C-746B-0F49-8B21-221411C8E693}" name="Budget" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{2781FA1C-8107-3A45-8365-873CEB86F752}" name="Actual" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{5529251C-746B-0F49-8B21-221411C8E693}" name="Budget" dataDxfId="30"/>
+    <tableColumn id="8" xr3:uid="{2781FA1C-8107-3A45-8365-873CEB86F752}" name="Actual" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6984,8 +7021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18BA6329-E680-5548-BB82-D6FB67EB7003}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fixed scroll bar format
</commit_message>
<xml_diff>
--- a/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
+++ b/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Managing Multiple Project Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A1E3B4-F0C8-5341-8F32-C74BA336F472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FADC2B9-A577-B245-A73F-D801D7EA2EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
+    <workbookView xWindow="8500" yWindow="760" windowWidth="24040" windowHeight="17420" activeTab="1" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="3" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="47">
   <si>
     <t>Project</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>Donut Chart</t>
+  </si>
+  <si>
+    <t>Scroll Bar</t>
   </si>
 </sst>
 </file>
@@ -4777,7 +4780,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="15" horiz="1" max="100" page="10" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="15" fmlaLink="Workings!$U$4" horiz="1" max="30" page="7"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7088,8 +7091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18BA6329-E680-5548-BB82-D6FB67EB7003}">
   <dimension ref="A1:AA49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8375,10 +8378,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F58449-19E8-9241-BC9F-FCB0CCBB3CD8}">
-  <dimension ref="B2:R6"/>
+  <dimension ref="B2:U6"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8391,7 +8394,7 @@
     <col min="18" max="18" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>35</v>
       </c>
@@ -8411,7 +8414,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B3">
         <f>COUNTIF(Dashboard!H9:H53, "="&amp;0)</f>
         <v>4</v>
@@ -8451,8 +8454,11 @@
       <c r="R3" t="s">
         <v>31</v>
       </c>
+      <c r="U3" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.2">
       <c r="I4" s="9" t="s">
         <v>34</v>
       </c>
@@ -8475,8 +8481,11 @@
       <c r="R4" s="11">
         <v>19695000</v>
       </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.2">
       <c r="P5" t="s">
         <v>45</v>
       </c>
@@ -8489,7 +8498,7 @@
         <v>0.57652749428789041</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B6" s="10"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed sequence cell format
</commit_message>
<xml_diff>
--- a/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
+++ b/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Managing Multiple Project Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71289FAB-7037-7643-9030-91609A91D951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE99E805-693A-7545-AE8C-8842DF600099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
   </bookViews>
@@ -288,17 +288,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -320,15 +320,123 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="38">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
@@ -6379,8 +6487,8 @@
     <dataField name="Budget " fld="8" baseField="0" baseItem="0" numFmtId="3"/>
     <dataField name="Actual " fld="9" baseField="0" baseItem="0" numFmtId="3"/>
   </dataFields>
-  <formats count="4">
-    <format dxfId="3">
+  <formats count="13">
+    <format dxfId="31">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6389,7 +6497,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="30">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6398,7 +6506,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="29">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6407,10 +6515,44 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="28">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="18">
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="16">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="14">
+      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
+    </format>
+    <format dxfId="12">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
+    </format>
+    <format dxfId="10">
+      <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
+    </format>
+    <format dxfId="8">
+      <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
+    </format>
+    <format dxfId="6">
+      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
+    </format>
+    <format dxfId="4">
+      <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
+    </format>
+    <format dxfId="2">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
             <x v="1"/>
           </reference>
         </references>
@@ -6649,17 +6791,17 @@
     <tableColumn id="1" xr3:uid="{73B096BE-E208-2142-8042-C8FF7EBE9CB4}" name="Project"/>
     <tableColumn id="2" xr3:uid="{9FEE26CA-FD34-8940-B511-23005FD52FD9}" name="Task"/>
     <tableColumn id="3" xr3:uid="{13477DA8-3E2B-9140-828B-5E4EEC4B192E}" name="Manager"/>
-    <tableColumn id="4" xr3:uid="{6F6235F3-DCA0-BE4A-80AD-F124C1F29DF7}" name="Start Date" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{6F6235F3-DCA0-BE4A-80AD-F124C1F29DF7}" name="Start Date" dataDxfId="37"/>
     <tableColumn id="5" xr3:uid="{906D9425-A9AF-D946-BD7E-AABF37A5C06F}" name="Duration"/>
-    <tableColumn id="9" xr3:uid="{49251E86-4677-9C41-8F83-14B60BE792A2}" name="End Date" dataDxfId="4">
+    <tableColumn id="9" xr3:uid="{49251E86-4677-9C41-8F83-14B60BE792A2}" name="End Date" dataDxfId="32">
       <calculatedColumnFormula>WORKDAY.INTL(Project_Data[[#This Row],[Start Date]]-1,Project_Data[[#This Row],[Duration]],7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5410ED6D-ABC2-B749-B761-98A3ACF6E8B5}" name="Days completed" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{1E1A1903-5E63-2C42-A785-7622E4CE1FFD}" name="Progress" dataDxfId="7">
+    <tableColumn id="10" xr3:uid="{5410ED6D-ABC2-B749-B761-98A3ACF6E8B5}" name="Days completed" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{1E1A1903-5E63-2C42-A785-7622E4CE1FFD}" name="Progress" dataDxfId="35">
       <calculatedColumnFormula>Project_Data[[#This Row],[Days completed]]/Project_Data[[#This Row],[Duration]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5529251C-746B-0F49-8B21-221411C8E693}" name="Budget" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{2781FA1C-8107-3A45-8365-873CEB86F752}" name="Actual" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{5529251C-746B-0F49-8B21-221411C8E693}" name="Budget" dataDxfId="34"/>
+    <tableColumn id="8" xr3:uid="{2781FA1C-8107-3A45-8365-873CEB86F752}" name="Actual" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6965,7 +7107,7 @@
   <dimension ref="A1:AA49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6981,7 +7123,7 @@
     <col min="31" max="16384" width="10.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="13" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" s="13" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>30</v>
       </c>
@@ -6991,85 +7133,87 @@
       </c>
       <c r="F1" s="14"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:27" s="20" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="17" cm="1">
+      <c r="K8" s="19" cm="1">
         <f t="array" ref="K8:Y8">_xlfn.SEQUENCE(1, 15, MIN(D9:D50)+Workings!U4,1)</f>
         <v>44609</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="19">
         <v>44610</v>
       </c>
-      <c r="M8" s="17">
+      <c r="M8" s="19">
         <v>44611</v>
       </c>
-      <c r="N8" s="17">
+      <c r="N8" s="19">
         <v>44612</v>
       </c>
-      <c r="O8" s="17">
+      <c r="O8" s="19">
         <v>44613</v>
       </c>
-      <c r="P8" s="17">
+      <c r="P8" s="19">
         <v>44614</v>
       </c>
-      <c r="Q8" s="17">
+      <c r="Q8" s="19">
         <v>44615</v>
       </c>
-      <c r="R8" s="17">
+      <c r="R8" s="19">
         <v>44616</v>
       </c>
-      <c r="S8" s="17">
+      <c r="S8" s="19">
         <v>44617</v>
       </c>
-      <c r="T8" s="17">
+      <c r="T8" s="19">
         <v>44618</v>
       </c>
-      <c r="U8" s="17">
+      <c r="U8" s="19">
         <v>44619</v>
       </c>
-      <c r="V8" s="17">
+      <c r="V8" s="19">
         <v>44620</v>
       </c>
-      <c r="W8" s="17">
+      <c r="W8" s="19">
         <v>44621</v>
       </c>
-      <c r="X8" s="17">
+      <c r="X8" s="19">
         <v>44622</v>
       </c>
-      <c r="Y8" s="17">
+      <c r="Y8" s="19">
         <v>44623</v>
       </c>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="5"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -7091,7 +7235,7 @@
       <c r="G9" s="3">
         <v>3</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="6">
         <v>0.375</v>
       </c>
       <c r="I9" s="3">
@@ -7101,7 +7245,7 @@
         <v>32256</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>13</v>
       </c>
@@ -7120,7 +7264,7 @@
       <c r="G10" s="3">
         <v>4</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="6">
         <v>0.44444444444444442</v>
       </c>
       <c r="I10" s="3">
@@ -7130,7 +7274,7 @@
         <v>226233</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -7149,7 +7293,7 @@
       <c r="G11" s="3">
         <v>3</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="6">
         <v>0.6</v>
       </c>
       <c r="I11" s="3">
@@ -7159,7 +7303,7 @@
         <v>401579</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>17</v>
       </c>
@@ -7178,7 +7322,7 @@
       <c r="G12" s="3">
         <v>3</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="6">
         <v>1</v>
       </c>
       <c r="I12" s="3">
@@ -7188,7 +7332,7 @@
         <v>807069</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>19</v>
       </c>
@@ -7207,7 +7351,7 @@
       <c r="G13" s="3">
         <v>3</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="6">
         <v>0.42857142857142855</v>
       </c>
       <c r="I13" s="3">
@@ -7217,7 +7361,7 @@
         <v>173166</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>21</v>
       </c>
@@ -7236,7 +7380,7 @@
       <c r="G14" s="3">
         <v>2</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="6">
         <v>0.2</v>
       </c>
       <c r="I14" s="3">
@@ -7246,7 +7390,7 @@
         <v>8400</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>22</v>
       </c>
@@ -7265,7 +7409,7 @@
       <c r="G15" s="3">
         <v>3</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="6">
         <v>0.3</v>
       </c>
       <c r="I15" s="3">
@@ -7275,7 +7419,7 @@
         <v>262679</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>23</v>
       </c>
@@ -7294,7 +7438,7 @@
       <c r="G16" s="3">
         <v>0</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16" s="6">
         <v>0</v>
       </c>
       <c r="I16" s="3">
@@ -7326,7 +7470,7 @@
       <c r="G17" s="3">
         <v>8</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17" s="6">
         <v>0.88888888888888884</v>
       </c>
       <c r="I17" s="3">
@@ -7355,7 +7499,7 @@
       <c r="G18" s="3">
         <v>2</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18" s="6">
         <v>0.2</v>
       </c>
       <c r="I18" s="3">
@@ -7384,7 +7528,7 @@
       <c r="G19" s="3">
         <v>0</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H19" s="6">
         <v>0</v>
       </c>
       <c r="I19" s="3">
@@ -7413,7 +7557,7 @@
       <c r="G20" s="3">
         <v>5</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20" s="6">
         <v>0.625</v>
       </c>
       <c r="I20" s="3">
@@ -7442,7 +7586,7 @@
       <c r="G21" s="3">
         <v>3</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21" s="6">
         <v>0.3</v>
       </c>
       <c r="I21" s="3">
@@ -7471,7 +7615,7 @@
       <c r="G22" s="3">
         <v>3</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22" s="6">
         <v>0.5</v>
       </c>
       <c r="I22" s="3">
@@ -7500,7 +7644,7 @@
       <c r="G23" s="3">
         <v>2</v>
       </c>
-      <c r="H23" s="5">
+      <c r="H23" s="6">
         <v>0.5</v>
       </c>
       <c r="I23" s="3">
@@ -7532,7 +7676,7 @@
       <c r="G24" s="3">
         <v>2</v>
       </c>
-      <c r="H24" s="5">
+      <c r="H24" s="6">
         <v>0.4</v>
       </c>
       <c r="I24" s="3">
@@ -7561,7 +7705,7 @@
       <c r="G25" s="3">
         <v>3</v>
       </c>
-      <c r="H25" s="5">
+      <c r="H25" s="6">
         <v>0.5</v>
       </c>
       <c r="I25" s="3">
@@ -7590,7 +7734,7 @@
       <c r="G26" s="3">
         <v>3</v>
       </c>
-      <c r="H26" s="5">
+      <c r="H26" s="6">
         <v>0.5</v>
       </c>
       <c r="I26" s="3">
@@ -7619,7 +7763,7 @@
       <c r="G27" s="3">
         <v>4</v>
       </c>
-      <c r="H27" s="5">
+      <c r="H27" s="6">
         <v>0.4</v>
       </c>
       <c r="I27" s="3">
@@ -7648,7 +7792,7 @@
       <c r="G28" s="3">
         <v>3</v>
       </c>
-      <c r="H28" s="5">
+      <c r="H28" s="6">
         <v>0.33333333333333331</v>
       </c>
       <c r="I28" s="3">
@@ -7677,7 +7821,7 @@
       <c r="G29" s="3">
         <v>1</v>
       </c>
-      <c r="H29" s="5">
+      <c r="H29" s="6">
         <v>0.25</v>
       </c>
       <c r="I29" s="3">
@@ -7706,7 +7850,7 @@
       <c r="G30" s="3">
         <v>0</v>
       </c>
-      <c r="H30" s="5">
+      <c r="H30" s="6">
         <v>0</v>
       </c>
       <c r="I30" s="3">
@@ -7735,7 +7879,7 @@
       <c r="G31" s="3">
         <v>3</v>
       </c>
-      <c r="H31" s="5">
+      <c r="H31" s="6">
         <v>0.42857142857142855</v>
       </c>
       <c r="I31" s="3">
@@ -7764,7 +7908,7 @@
       <c r="G32" s="3">
         <v>2</v>
       </c>
-      <c r="H32" s="5">
+      <c r="H32" s="6">
         <v>0.4</v>
       </c>
       <c r="I32" s="3">
@@ -7793,7 +7937,7 @@
       <c r="G33" s="3">
         <v>1</v>
       </c>
-      <c r="H33" s="5">
+      <c r="H33" s="6">
         <v>0.1111111111111111</v>
       </c>
       <c r="I33" s="3">
@@ -7825,7 +7969,7 @@
       <c r="G34" s="3">
         <v>7</v>
       </c>
-      <c r="H34" s="5">
+      <c r="H34" s="6">
         <v>1</v>
       </c>
       <c r="I34" s="3">
@@ -7854,7 +7998,7 @@
       <c r="G35" s="3">
         <v>3</v>
       </c>
-      <c r="H35" s="5">
+      <c r="H35" s="6">
         <v>1</v>
       </c>
       <c r="I35" s="3">
@@ -7883,7 +8027,7 @@
       <c r="G36" s="3">
         <v>4</v>
       </c>
-      <c r="H36" s="5">
+      <c r="H36" s="6">
         <v>0.44444444444444442</v>
       </c>
       <c r="I36" s="3">
@@ -7912,7 +8056,7 @@
       <c r="G37" s="3">
         <v>0</v>
       </c>
-      <c r="H37" s="5">
+      <c r="H37" s="6">
         <v>0</v>
       </c>
       <c r="I37" s="3">
@@ -7941,7 +8085,7 @@
       <c r="G38" s="3">
         <v>3</v>
       </c>
-      <c r="H38" s="5">
+      <c r="H38" s="6">
         <v>0.42857142857142855</v>
       </c>
       <c r="I38" s="3">
@@ -7970,7 +8114,7 @@
       <c r="G39" s="3">
         <v>1</v>
       </c>
-      <c r="H39" s="5">
+      <c r="H39" s="6">
         <v>0.25</v>
       </c>
       <c r="I39" s="3">
@@ -7999,7 +8143,7 @@
       <c r="G40" s="3">
         <v>3</v>
       </c>
-      <c r="H40" s="5">
+      <c r="H40" s="6">
         <v>0.5</v>
       </c>
       <c r="I40" s="3">
@@ -8028,7 +8172,7 @@
       <c r="G41" s="3">
         <v>5</v>
       </c>
-      <c r="H41" s="5">
+      <c r="H41" s="6">
         <v>0.83333333333333337</v>
       </c>
       <c r="I41" s="3">
@@ -8057,7 +8201,7 @@
       <c r="G42" s="3">
         <v>1</v>
       </c>
-      <c r="H42" s="5">
+      <c r="H42" s="6">
         <v>0.25</v>
       </c>
       <c r="I42" s="3">
@@ -8086,7 +8230,7 @@
       <c r="G43" s="3">
         <v>3</v>
       </c>
-      <c r="H43" s="5">
+      <c r="H43" s="6">
         <v>0.42857142857142855</v>
       </c>
       <c r="I43" s="3">
@@ -8118,7 +8262,7 @@
       <c r="G44" s="3">
         <v>5</v>
       </c>
-      <c r="H44" s="5">
+      <c r="H44" s="6">
         <v>0.5</v>
       </c>
       <c r="I44" s="3">
@@ -8147,7 +8291,7 @@
       <c r="G45" s="3">
         <v>4</v>
       </c>
-      <c r="H45" s="5">
+      <c r="H45" s="6">
         <v>0.8</v>
       </c>
       <c r="I45" s="3">
@@ -8176,7 +8320,7 @@
       <c r="G46" s="3">
         <v>3</v>
       </c>
-      <c r="H46" s="5">
+      <c r="H46" s="6">
         <v>0.42857142857142855</v>
       </c>
       <c r="I46" s="3">
@@ -8205,7 +8349,7 @@
       <c r="G47" s="3">
         <v>2</v>
       </c>
-      <c r="H47" s="5">
+      <c r="H47" s="6">
         <v>0.2857142857142857</v>
       </c>
       <c r="I47" s="3">
@@ -8234,7 +8378,7 @@
       <c r="G48" s="3">
         <v>2</v>
       </c>
-      <c r="H48" s="5">
+      <c r="H48" s="6">
         <v>0.66666666666666663</v>
       </c>
       <c r="I48" s="3">
@@ -8257,7 +8401,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H9:H50">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -8268,6 +8412,11 @@
           <x14:id>{29E0FBCC-2B8A-7E47-B182-DD695C7DF8FE}</x14:id>
         </ext>
       </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K8:Y8">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$K8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8360,7 +8509,7 @@
       <c r="F2" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added weekend to sequence chart
</commit_message>
<xml_diff>
--- a/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
+++ b/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Managing Multiple Project Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8667A529-BCA6-3240-9FD0-29EE9F932940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D6F181-A87D-B84D-86C2-8123E133E7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
   </bookViews>
@@ -338,7 +338,197 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="39">
+  <dxfs count="54">
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkGray">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <alignment vertical="center"/>
     </dxf>
@@ -395,23 +585,6 @@
     </dxf>
     <dxf>
       <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <fill>
@@ -6505,7 +6678,7 @@
     <dataField name="Actual " fld="9" baseField="0" baseItem="0" numFmtId="3"/>
   </dataFields>
   <formats count="31">
-    <format dxfId="32">
+    <format dxfId="47">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6514,7 +6687,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="46">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6523,7 +6696,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="45">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6532,7 +6705,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="44">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6541,55 +6714,55 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="43">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="27">
+    <format dxfId="42">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="26">
+    <format dxfId="41">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="25">
+    <format dxfId="40">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="24">
+    <format dxfId="39">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="23">
+    <format dxfId="38">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="22">
+    <format dxfId="37">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="21">
+    <format dxfId="36">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="18">
+    <format dxfId="34">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="17">
+    <format dxfId="33">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="16">
+    <format dxfId="32">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="15">
+    <format dxfId="31">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="14">
+    <format dxfId="30">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="13">
+    <format dxfId="29">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="12">
+    <format dxfId="28">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="11">
+    <format dxfId="27">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="10">
+    <format dxfId="26">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -6599,31 +6772,31 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="25">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="8">
+    <format dxfId="24">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="7">
+    <format dxfId="23">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="22">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="5">
+    <format dxfId="21">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="20">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="3">
+    <format dxfId="19">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="18">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="1">
+    <format dxfId="17">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -6633,7 +6806,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="16">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -6876,17 +7049,17 @@
     <tableColumn id="1" xr3:uid="{73B096BE-E208-2142-8042-C8FF7EBE9CB4}" name="Project"/>
     <tableColumn id="2" xr3:uid="{9FEE26CA-FD34-8940-B511-23005FD52FD9}" name="Task"/>
     <tableColumn id="3" xr3:uid="{13477DA8-3E2B-9140-828B-5E4EEC4B192E}" name="Manager"/>
-    <tableColumn id="4" xr3:uid="{6F6235F3-DCA0-BE4A-80AD-F124C1F29DF7}" name="Start Date" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{6F6235F3-DCA0-BE4A-80AD-F124C1F29DF7}" name="Start Date" dataDxfId="53"/>
     <tableColumn id="5" xr3:uid="{906D9425-A9AF-D946-BD7E-AABF37A5C06F}" name="Duration"/>
-    <tableColumn id="9" xr3:uid="{49251E86-4677-9C41-8F83-14B60BE792A2}" name="End Date" dataDxfId="33">
+    <tableColumn id="9" xr3:uid="{49251E86-4677-9C41-8F83-14B60BE792A2}" name="End Date" dataDxfId="48">
       <calculatedColumnFormula>WORKDAY.INTL(Project_Data[[#This Row],[Start Date]]-1,Project_Data[[#This Row],[Duration]],7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5410ED6D-ABC2-B749-B761-98A3ACF6E8B5}" name="Days completed" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{1E1A1903-5E63-2C42-A785-7622E4CE1FFD}" name="Progress" dataDxfId="36">
+    <tableColumn id="10" xr3:uid="{5410ED6D-ABC2-B749-B761-98A3ACF6E8B5}" name="Days completed" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{1E1A1903-5E63-2C42-A785-7622E4CE1FFD}" name="Progress" dataDxfId="51">
       <calculatedColumnFormula>Project_Data[[#This Row],[Days completed]]/Project_Data[[#This Row],[Duration]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5529251C-746B-0F49-8B21-221411C8E693}" name="Budget" dataDxfId="35"/>
-    <tableColumn id="8" xr3:uid="{2781FA1C-8107-3A45-8365-873CEB86F752}" name="Actual" dataDxfId="34"/>
+    <tableColumn id="7" xr3:uid="{5529251C-746B-0F49-8B21-221411C8E693}" name="Budget" dataDxfId="50"/>
+    <tableColumn id="8" xr3:uid="{2781FA1C-8107-3A45-8365-873CEB86F752}" name="Actual" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7191,9 +7364,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18BA6329-E680-5548-BB82-D6FB67EB7003}">
   <dimension ref="A1:AA49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N14" sqref="N14"/>
+      <selection pane="bottomLeft" activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8487,7 +8660,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H9:H50">
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -8501,8 +8674,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:Y8">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$K8&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9:Y50">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>AND(WEEKDAY(K$8,17)&gt;5, $B9&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added in progress formatting
</commit_message>
<xml_diff>
--- a/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
+++ b/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Managing Multiple Project Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D6F181-A87D-B84D-86C2-8123E133E7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1723612-9046-1442-958B-341D039710E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
   </bookViews>
@@ -338,10 +338,68 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="54">
+  <dxfs count="60">
     <dxf>
       <fill>
-        <patternFill patternType="mediumGray">
+        <patternFill>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkGray">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8A84"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkGray">
           <bgColor auto="1"/>
         </patternFill>
       </fill>
@@ -366,6 +424,30 @@
     <dxf>
       <fill>
         <patternFill patternType="darkGray">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
           <bgColor auto="1"/>
         </patternFill>
       </fill>
@@ -6678,7 +6760,7 @@
     <dataField name="Actual " fld="9" baseField="0" baseItem="0" numFmtId="3"/>
   </dataFields>
   <formats count="31">
-    <format dxfId="47">
+    <format dxfId="53">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6687,7 +6769,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="46">
+    <format dxfId="52">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6696,7 +6778,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="45">
+    <format dxfId="51">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6705,7 +6787,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="44">
+    <format dxfId="50">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6714,55 +6796,55 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="43">
+    <format dxfId="49">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="42">
+    <format dxfId="48">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="41">
+    <format dxfId="47">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="40">
+    <format dxfId="46">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="39">
+    <format dxfId="45">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="38">
+    <format dxfId="44">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="37">
+    <format dxfId="43">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="36">
+    <format dxfId="42">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="34">
+    <format dxfId="40">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="33">
+    <format dxfId="39">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="32">
+    <format dxfId="38">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="31">
+    <format dxfId="37">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="30">
+    <format dxfId="36">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="29">
+    <format dxfId="35">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="28">
+    <format dxfId="34">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="27">
+    <format dxfId="33">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="26">
+    <format dxfId="32">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -6772,31 +6854,31 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="31">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="24">
+    <format dxfId="30">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="23">
+    <format dxfId="29">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="22">
+    <format dxfId="28">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="21">
+    <format dxfId="27">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="20">
+    <format dxfId="26">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="19">
+    <format dxfId="25">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="18">
+    <format dxfId="24">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="17">
+    <format dxfId="23">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -6806,7 +6888,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="22">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -7049,17 +7131,17 @@
     <tableColumn id="1" xr3:uid="{73B096BE-E208-2142-8042-C8FF7EBE9CB4}" name="Project"/>
     <tableColumn id="2" xr3:uid="{9FEE26CA-FD34-8940-B511-23005FD52FD9}" name="Task"/>
     <tableColumn id="3" xr3:uid="{13477DA8-3E2B-9140-828B-5E4EEC4B192E}" name="Manager"/>
-    <tableColumn id="4" xr3:uid="{6F6235F3-DCA0-BE4A-80AD-F124C1F29DF7}" name="Start Date" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{6F6235F3-DCA0-BE4A-80AD-F124C1F29DF7}" name="Start Date" dataDxfId="59"/>
     <tableColumn id="5" xr3:uid="{906D9425-A9AF-D946-BD7E-AABF37A5C06F}" name="Duration"/>
-    <tableColumn id="9" xr3:uid="{49251E86-4677-9C41-8F83-14B60BE792A2}" name="End Date" dataDxfId="48">
+    <tableColumn id="9" xr3:uid="{49251E86-4677-9C41-8F83-14B60BE792A2}" name="End Date" dataDxfId="54">
       <calculatedColumnFormula>WORKDAY.INTL(Project_Data[[#This Row],[Start Date]]-1,Project_Data[[#This Row],[Duration]],7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5410ED6D-ABC2-B749-B761-98A3ACF6E8B5}" name="Days completed" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{1E1A1903-5E63-2C42-A785-7622E4CE1FFD}" name="Progress" dataDxfId="51">
+    <tableColumn id="10" xr3:uid="{5410ED6D-ABC2-B749-B761-98A3ACF6E8B5}" name="Days completed" dataDxfId="58"/>
+    <tableColumn id="6" xr3:uid="{1E1A1903-5E63-2C42-A785-7622E4CE1FFD}" name="Progress" dataDxfId="57">
       <calculatedColumnFormula>Project_Data[[#This Row],[Days completed]]/Project_Data[[#This Row],[Duration]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5529251C-746B-0F49-8B21-221411C8E693}" name="Budget" dataDxfId="50"/>
-    <tableColumn id="8" xr3:uid="{2781FA1C-8107-3A45-8365-873CEB86F752}" name="Actual" dataDxfId="49"/>
+    <tableColumn id="7" xr3:uid="{5529251C-746B-0F49-8B21-221411C8E693}" name="Budget" dataDxfId="56"/>
+    <tableColumn id="8" xr3:uid="{2781FA1C-8107-3A45-8365-873CEB86F752}" name="Actual" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7366,7 +7448,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W17" sqref="W17"/>
+      <selection pane="bottomLeft" activeCell="Y24" sqref="Y24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8660,7 +8742,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H9:H50">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -8674,13 +8756,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:Y8">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>$K8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:Y50">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>AND(WEEKDAY(K$8,17)&gt;5, $B9&lt;&gt;"")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>AND(K$8 &gt;= $D9, WORKDAY.INTL($D9, $G9, 7)-1 &gt;= K$8)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Formatted in progress days
</commit_message>
<xml_diff>
--- a/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
+++ b/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Managing Multiple Project Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1723612-9046-1442-958B-341D039710E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD74F1E-4DB7-8C44-B77E-8F5C02E0D1D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
+    <workbookView xWindow="20" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="3" r:id="rId1"/>
@@ -338,11 +338,94 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="60">
+  <dxfs count="68">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF8A84"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="8"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkGray">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF8A84"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
         </patternFill>
       </fill>
       <border>
@@ -384,6 +467,47 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF8A84"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkGray">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8"/>
         </patternFill>
       </fill>
       <border>
@@ -6760,7 +6884,7 @@
     <dataField name="Actual " fld="9" baseField="0" baseItem="0" numFmtId="3"/>
   </dataFields>
   <formats count="31">
-    <format dxfId="53">
+    <format dxfId="61">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6769,7 +6893,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="52">
+    <format dxfId="60">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6778,7 +6902,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="51">
+    <format dxfId="59">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6787,7 +6911,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="50">
+    <format dxfId="58">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6796,55 +6920,55 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="49">
+    <format dxfId="57">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="48">
+    <format dxfId="56">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="47">
+    <format dxfId="55">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="46">
+    <format dxfId="54">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="45">
+    <format dxfId="53">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="44">
+    <format dxfId="52">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="43">
+    <format dxfId="51">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
+    <format dxfId="50">
+      <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
+    </format>
+    <format dxfId="48">
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="47">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="46">
+      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
+    </format>
+    <format dxfId="45">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
+    </format>
+    <format dxfId="44">
+      <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
+    </format>
+    <format dxfId="43">
+      <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
+    </format>
     <format dxfId="42">
+      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
+    </format>
+    <format dxfId="41">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
     <format dxfId="40">
-      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="39">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
-    </format>
-    <format dxfId="38">
-      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
-    </format>
-    <format dxfId="37">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
-    </format>
-    <format dxfId="36">
-      <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
-    </format>
-    <format dxfId="35">
-      <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
-    </format>
-    <format dxfId="34">
-      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
-    </format>
-    <format dxfId="33">
-      <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
-    </format>
-    <format dxfId="32">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -6854,31 +6978,31 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="39">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="30">
+    <format dxfId="38">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="29">
+    <format dxfId="37">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="28">
+    <format dxfId="36">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="27">
+    <format dxfId="35">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="26">
+    <format dxfId="34">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="25">
+    <format dxfId="33">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="24">
+    <format dxfId="32">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="23">
+    <format dxfId="31">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -6888,7 +7012,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="22">
+    <format dxfId="30">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -7131,17 +7255,17 @@
     <tableColumn id="1" xr3:uid="{73B096BE-E208-2142-8042-C8FF7EBE9CB4}" name="Project"/>
     <tableColumn id="2" xr3:uid="{9FEE26CA-FD34-8940-B511-23005FD52FD9}" name="Task"/>
     <tableColumn id="3" xr3:uid="{13477DA8-3E2B-9140-828B-5E4EEC4B192E}" name="Manager"/>
-    <tableColumn id="4" xr3:uid="{6F6235F3-DCA0-BE4A-80AD-F124C1F29DF7}" name="Start Date" dataDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{6F6235F3-DCA0-BE4A-80AD-F124C1F29DF7}" name="Start Date" dataDxfId="67"/>
     <tableColumn id="5" xr3:uid="{906D9425-A9AF-D946-BD7E-AABF37A5C06F}" name="Duration"/>
-    <tableColumn id="9" xr3:uid="{49251E86-4677-9C41-8F83-14B60BE792A2}" name="End Date" dataDxfId="54">
+    <tableColumn id="9" xr3:uid="{49251E86-4677-9C41-8F83-14B60BE792A2}" name="End Date" dataDxfId="62">
       <calculatedColumnFormula>WORKDAY.INTL(Project_Data[[#This Row],[Start Date]]-1,Project_Data[[#This Row],[Duration]],7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5410ED6D-ABC2-B749-B761-98A3ACF6E8B5}" name="Days completed" dataDxfId="58"/>
-    <tableColumn id="6" xr3:uid="{1E1A1903-5E63-2C42-A785-7622E4CE1FFD}" name="Progress" dataDxfId="57">
+    <tableColumn id="10" xr3:uid="{5410ED6D-ABC2-B749-B761-98A3ACF6E8B5}" name="Days completed" dataDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{1E1A1903-5E63-2C42-A785-7622E4CE1FFD}" name="Progress" dataDxfId="65">
       <calculatedColumnFormula>Project_Data[[#This Row],[Days completed]]/Project_Data[[#This Row],[Duration]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5529251C-746B-0F49-8B21-221411C8E693}" name="Budget" dataDxfId="56"/>
-    <tableColumn id="8" xr3:uid="{2781FA1C-8107-3A45-8365-873CEB86F752}" name="Actual" dataDxfId="55"/>
+    <tableColumn id="7" xr3:uid="{5529251C-746B-0F49-8B21-221411C8E693}" name="Budget" dataDxfId="64"/>
+    <tableColumn id="8" xr3:uid="{2781FA1C-8107-3A45-8365-873CEB86F752}" name="Actual" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7448,7 +7572,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y24" sqref="Y24"/>
+      <selection pane="bottomLeft" activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8742,7 +8866,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H9:H50">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -8756,16 +8880,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:Y8">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>$K8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:Y50">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>AND(WEEKDAY(K$8,17)&gt;5, $B9&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>AND(K$8 &gt;= $D9, WORKDAY.INTL($D9, $G9, 7)-1 &gt;= K$8)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>AND(K$8 &gt;= WORKDAY.INTL($D9, $G9, 7), $H9 &lt;&gt; 1, K$8 &lt;= $E9)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Formatted not completed bars
</commit_message>
<xml_diff>
--- a/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
+++ b/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Managing Multiple Project Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD74F1E-4DB7-8C44-B77E-8F5C02E0D1D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD28D7D8-1C1A-7045-B478-5AF11B940198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
   </bookViews>
@@ -338,7 +338,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="68">
+  <dxfs count="73">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -346,12 +346,8 @@
         </patternFill>
       </fill>
       <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
+        <left/>
+        <right/>
         <top style="thin">
           <color theme="0"/>
         </top>
@@ -404,6 +400,48 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFFF8A84"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFF8A84"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFF8A84"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFFF8A84"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkGray">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FFFF8A84"/>
@@ -412,6 +450,46 @@
       <border>
         <left/>
         <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF8A84"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
         <top style="thin">
           <color theme="0"/>
         </top>
@@ -6884,7 +6962,7 @@
     <dataField name="Actual " fld="9" baseField="0" baseItem="0" numFmtId="3"/>
   </dataFields>
   <formats count="31">
-    <format dxfId="61">
+    <format dxfId="66">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6893,7 +6971,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="60">
+    <format dxfId="65">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6902,7 +6980,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="59">
+    <format dxfId="64">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6911,7 +6989,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="58">
+    <format dxfId="63">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6920,55 +6998,55 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="57">
+    <format dxfId="62">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="56">
+    <format dxfId="61">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="55">
+    <format dxfId="60">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="54">
+    <format dxfId="59">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="53">
+    <format dxfId="58">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="52">
+    <format dxfId="57">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="51">
+    <format dxfId="56">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="50">
+    <format dxfId="55">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="48">
+    <format dxfId="53">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="47">
+    <format dxfId="52">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="46">
+    <format dxfId="51">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="45">
+    <format dxfId="50">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="44">
+    <format dxfId="49">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="43">
+    <format dxfId="48">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="42">
+    <format dxfId="47">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="41">
+    <format dxfId="46">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="40">
+    <format dxfId="45">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -6978,31 +7056,31 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="39">
+    <format dxfId="44">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="38">
+    <format dxfId="43">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="37">
+    <format dxfId="42">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="36">
+    <format dxfId="41">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="35">
+    <format dxfId="40">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="34">
+    <format dxfId="39">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="33">
+    <format dxfId="38">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="32">
+    <format dxfId="37">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="31">
+    <format dxfId="36">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -7012,7 +7090,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="35">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -7255,17 +7333,17 @@
     <tableColumn id="1" xr3:uid="{73B096BE-E208-2142-8042-C8FF7EBE9CB4}" name="Project"/>
     <tableColumn id="2" xr3:uid="{9FEE26CA-FD34-8940-B511-23005FD52FD9}" name="Task"/>
     <tableColumn id="3" xr3:uid="{13477DA8-3E2B-9140-828B-5E4EEC4B192E}" name="Manager"/>
-    <tableColumn id="4" xr3:uid="{6F6235F3-DCA0-BE4A-80AD-F124C1F29DF7}" name="Start Date" dataDxfId="67"/>
+    <tableColumn id="4" xr3:uid="{6F6235F3-DCA0-BE4A-80AD-F124C1F29DF7}" name="Start Date" dataDxfId="72"/>
     <tableColumn id="5" xr3:uid="{906D9425-A9AF-D946-BD7E-AABF37A5C06F}" name="Duration"/>
-    <tableColumn id="9" xr3:uid="{49251E86-4677-9C41-8F83-14B60BE792A2}" name="End Date" dataDxfId="62">
+    <tableColumn id="9" xr3:uid="{49251E86-4677-9C41-8F83-14B60BE792A2}" name="End Date" dataDxfId="67">
       <calculatedColumnFormula>WORKDAY.INTL(Project_Data[[#This Row],[Start Date]]-1,Project_Data[[#This Row],[Duration]],7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5410ED6D-ABC2-B749-B761-98A3ACF6E8B5}" name="Days completed" dataDxfId="66"/>
-    <tableColumn id="6" xr3:uid="{1E1A1903-5E63-2C42-A785-7622E4CE1FFD}" name="Progress" dataDxfId="65">
+    <tableColumn id="10" xr3:uid="{5410ED6D-ABC2-B749-B761-98A3ACF6E8B5}" name="Days completed" dataDxfId="71"/>
+    <tableColumn id="6" xr3:uid="{1E1A1903-5E63-2C42-A785-7622E4CE1FFD}" name="Progress" dataDxfId="70">
       <calculatedColumnFormula>Project_Data[[#This Row],[Days completed]]/Project_Data[[#This Row],[Duration]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5529251C-746B-0F49-8B21-221411C8E693}" name="Budget" dataDxfId="64"/>
-    <tableColumn id="8" xr3:uid="{2781FA1C-8107-3A45-8365-873CEB86F752}" name="Actual" dataDxfId="63"/>
+    <tableColumn id="7" xr3:uid="{5529251C-746B-0F49-8B21-221411C8E693}" name="Budget" dataDxfId="69"/>
+    <tableColumn id="8" xr3:uid="{2781FA1C-8107-3A45-8365-873CEB86F752}" name="Actual" dataDxfId="68"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7572,7 +7650,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U10" sqref="U10"/>
+      <selection pane="bottomLeft" activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8866,7 +8944,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H9:H50">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -8880,19 +8958,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:Y8">
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>$K8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:Y50">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>AND(WEEKDAY(K$8,17)&gt;5, $B9&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>AND(K$8 &gt;= $D9, WORKDAY.INTL($D9, $G9, 7)-1 &gt;= K$8)</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="7" priority="2">
+      <formula>AND(K$8 &gt;= WORKDAY.INTL($D9, $G9, 7), $H9 &lt;&gt; 1, K$8 &lt;= $E9)</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="4" priority="1">
-      <formula>AND(K$8 &gt;= WORKDAY.INTL($D9, $G9, 7), $H9 &lt;&gt; 1, K$8 &lt;= $E9)</formula>
+      <formula>"and(k$8 &gt;= workday.intl($D9, $G9, 7), $H9=0, K$8 &lt;= $E9)"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed not started formating
</commit_message>
<xml_diff>
--- a/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
+++ b/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Managing Multiple Project Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD28D7D8-1C1A-7045-B478-5AF11B940198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D15FFC6-513F-6245-A187-B930491E0CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
   </bookViews>
@@ -338,7 +338,25 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="73">
+  <dxfs count="88">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFFF8A84"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFF8A84"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFF8A84"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFFF8A84"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -419,10 +437,22 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="darkGray">
-          <bgColor auto="1"/>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF8A84"/>
         </patternFill>
       </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -436,6 +466,48 @@
         </top>
         <bottom style="thin">
           <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkGray">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFFF8A84"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFF8A84"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFF8A84"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFFF8A84"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -459,6 +531,168 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkGray">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFFF8A84"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFF8A84"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFF8A84"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFFF8A84"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF8A84"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkGray">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF8A84"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkGray">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -6962,7 +7196,7 @@
     <dataField name="Actual " fld="9" baseField="0" baseItem="0" numFmtId="3"/>
   </dataFields>
   <formats count="31">
-    <format dxfId="66">
+    <format dxfId="81">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6971,7 +7205,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="65">
+    <format dxfId="80">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6980,7 +7214,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="64">
+    <format dxfId="79">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6989,7 +7223,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="63">
+    <format dxfId="78">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -6998,55 +7232,55 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="62">
+    <format dxfId="77">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="61">
+    <format dxfId="76">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="60">
+    <format dxfId="75">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="59">
+    <format dxfId="74">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="58">
+    <format dxfId="73">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="57">
+    <format dxfId="72">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="56">
+    <format dxfId="71">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="55">
+    <format dxfId="70">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="53">
+    <format dxfId="68">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="52">
+    <format dxfId="67">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="51">
+    <format dxfId="66">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="50">
+    <format dxfId="65">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="49">
+    <format dxfId="64">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="48">
+    <format dxfId="63">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="47">
+    <format dxfId="62">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="46">
+    <format dxfId="61">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="45">
+    <format dxfId="60">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -7056,31 +7290,31 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="44">
+    <format dxfId="59">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="43">
+    <format dxfId="58">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="42">
+    <format dxfId="57">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="41">
+    <format dxfId="56">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="40">
+    <format dxfId="55">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="39">
+    <format dxfId="54">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="38">
+    <format dxfId="53">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="37">
+    <format dxfId="52">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="36">
+    <format dxfId="51">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -7090,7 +7324,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="35">
+    <format dxfId="50">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -7333,17 +7567,17 @@
     <tableColumn id="1" xr3:uid="{73B096BE-E208-2142-8042-C8FF7EBE9CB4}" name="Project"/>
     <tableColumn id="2" xr3:uid="{9FEE26CA-FD34-8940-B511-23005FD52FD9}" name="Task"/>
     <tableColumn id="3" xr3:uid="{13477DA8-3E2B-9140-828B-5E4EEC4B192E}" name="Manager"/>
-    <tableColumn id="4" xr3:uid="{6F6235F3-DCA0-BE4A-80AD-F124C1F29DF7}" name="Start Date" dataDxfId="72"/>
+    <tableColumn id="4" xr3:uid="{6F6235F3-DCA0-BE4A-80AD-F124C1F29DF7}" name="Start Date" dataDxfId="87"/>
     <tableColumn id="5" xr3:uid="{906D9425-A9AF-D946-BD7E-AABF37A5C06F}" name="Duration"/>
-    <tableColumn id="9" xr3:uid="{49251E86-4677-9C41-8F83-14B60BE792A2}" name="End Date" dataDxfId="67">
+    <tableColumn id="9" xr3:uid="{49251E86-4677-9C41-8F83-14B60BE792A2}" name="End Date" dataDxfId="82">
       <calculatedColumnFormula>WORKDAY.INTL(Project_Data[[#This Row],[Start Date]]-1,Project_Data[[#This Row],[Duration]],7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5410ED6D-ABC2-B749-B761-98A3ACF6E8B5}" name="Days completed" dataDxfId="71"/>
-    <tableColumn id="6" xr3:uid="{1E1A1903-5E63-2C42-A785-7622E4CE1FFD}" name="Progress" dataDxfId="70">
+    <tableColumn id="10" xr3:uid="{5410ED6D-ABC2-B749-B761-98A3ACF6E8B5}" name="Days completed" dataDxfId="86"/>
+    <tableColumn id="6" xr3:uid="{1E1A1903-5E63-2C42-A785-7622E4CE1FFD}" name="Progress" dataDxfId="85">
       <calculatedColumnFormula>Project_Data[[#This Row],[Days completed]]/Project_Data[[#This Row],[Duration]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5529251C-746B-0F49-8B21-221411C8E693}" name="Budget" dataDxfId="69"/>
-    <tableColumn id="8" xr3:uid="{2781FA1C-8107-3A45-8365-873CEB86F752}" name="Actual" dataDxfId="68"/>
+    <tableColumn id="7" xr3:uid="{5529251C-746B-0F49-8B21-221411C8E693}" name="Budget" dataDxfId="84"/>
+    <tableColumn id="8" xr3:uid="{2781FA1C-8107-3A45-8365-873CEB86F752}" name="Actual" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7650,7 +7884,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X12" sqref="X12"/>
+      <selection pane="bottomLeft" activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8958,22 +9192,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:Y8">
-    <cfRule type="expression" dxfId="8" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>$K8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:Y50">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
       <formula>AND(WEEKDAY(K$8,17)&gt;5, $B9&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>AND(K$8 &gt;= $D9, WORKDAY.INTL($D9, $G9, 7)-1 &gt;= K$8)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>AND(K$8 &gt;= WORKDAY.INTL($D9, $G9, 7), $H9 &lt;&gt; 1, K$8 &lt;= $E9)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="1">
-      <formula>"and(k$8 &gt;= workday.intl($D9, $G9, 7), $H9=0, K$8 &lt;= $E9)"</formula>
+    <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
+      <formula>AND(K$8 &gt;= WORKDAY.INTL($D9, $G9, 7), $H9=0, K$8 &lt;= $E9)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Formatted grand total row
</commit_message>
<xml_diff>
--- a/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
+++ b/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Managing Multiple Project Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D15FFC6-513F-6245-A187-B930491E0CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26AC642-1CBF-C149-9EDC-5F7592EC39D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
+    <workbookView xWindow="12120" yWindow="760" windowWidth="18140" windowHeight="17420" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="3" r:id="rId1"/>
@@ -338,7 +338,283 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="88">
+  <dxfs count="106">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFFF8A84"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFF8A84"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFF8A84"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFFF8A84"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF8A84"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkGray">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFFF8A84"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFF8A84"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFF8A84"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFFF8A84"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF8A84"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkGray">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFFF8A84"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFFF8A84"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFFF8A84"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFFF8A84"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF8A84"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkGray">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -7196,7 +7472,7 @@
     <dataField name="Actual " fld="9" baseField="0" baseItem="0" numFmtId="3"/>
   </dataFields>
   <formats count="31">
-    <format dxfId="81">
+    <format dxfId="99">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -7205,7 +7481,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="80">
+    <format dxfId="98">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -7214,7 +7490,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="79">
+    <format dxfId="97">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -7223,10 +7499,68 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="78">
+    <format dxfId="96">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="95">
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="94">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="93">
+      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
+    </format>
+    <format dxfId="92">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
+    </format>
+    <format dxfId="91">
+      <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
+    </format>
+    <format dxfId="90">
+      <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
+    </format>
+    <format dxfId="89">
+      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
+    </format>
+    <format dxfId="88">
+      <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
+    </format>
+    <format dxfId="86">
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="85">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="84">
+      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
+    </format>
+    <format dxfId="83">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
+    </format>
+    <format dxfId="82">
+      <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
+    </format>
+    <format dxfId="81">
+      <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
+    </format>
+    <format dxfId="80">
+      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
+    </format>
+    <format dxfId="79">
+      <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
+    </format>
+    <format dxfId="78">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
             <x v="1"/>
           </reference>
         </references>
@@ -7256,31 +7590,7 @@
     <format dxfId="70">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="68">
-      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="67">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
-    </format>
-    <format dxfId="66">
-      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
-    </format>
-    <format dxfId="65">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
-    </format>
-    <format dxfId="64">
-      <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
-    </format>
-    <format dxfId="63">
-      <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
-    </format>
-    <format dxfId="62">
-      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
-    </format>
-    <format dxfId="61">
-      <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
-    </format>
-    <format dxfId="60">
+    <format dxfId="69">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -7290,41 +7600,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="59">
-      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="58">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
-    </format>
-    <format dxfId="57">
-      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
-    </format>
-    <format dxfId="56">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
-    </format>
-    <format dxfId="55">
-      <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
-    </format>
-    <format dxfId="54">
-      <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
-    </format>
-    <format dxfId="53">
-      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
-    </format>
-    <format dxfId="52">
-      <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
-    </format>
-    <format dxfId="51">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="2">
-            <x v="0"/>
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="50">
+    <format dxfId="68">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -7567,17 +7843,17 @@
     <tableColumn id="1" xr3:uid="{73B096BE-E208-2142-8042-C8FF7EBE9CB4}" name="Project"/>
     <tableColumn id="2" xr3:uid="{9FEE26CA-FD34-8940-B511-23005FD52FD9}" name="Task"/>
     <tableColumn id="3" xr3:uid="{13477DA8-3E2B-9140-828B-5E4EEC4B192E}" name="Manager"/>
-    <tableColumn id="4" xr3:uid="{6F6235F3-DCA0-BE4A-80AD-F124C1F29DF7}" name="Start Date" dataDxfId="87"/>
+    <tableColumn id="4" xr3:uid="{6F6235F3-DCA0-BE4A-80AD-F124C1F29DF7}" name="Start Date" dataDxfId="105"/>
     <tableColumn id="5" xr3:uid="{906D9425-A9AF-D946-BD7E-AABF37A5C06F}" name="Duration"/>
-    <tableColumn id="9" xr3:uid="{49251E86-4677-9C41-8F83-14B60BE792A2}" name="End Date" dataDxfId="82">
+    <tableColumn id="9" xr3:uid="{49251E86-4677-9C41-8F83-14B60BE792A2}" name="End Date" dataDxfId="100">
       <calculatedColumnFormula>WORKDAY.INTL(Project_Data[[#This Row],[Start Date]]-1,Project_Data[[#This Row],[Duration]],7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5410ED6D-ABC2-B749-B761-98A3ACF6E8B5}" name="Days completed" dataDxfId="86"/>
-    <tableColumn id="6" xr3:uid="{1E1A1903-5E63-2C42-A785-7622E4CE1FFD}" name="Progress" dataDxfId="85">
+    <tableColumn id="10" xr3:uid="{5410ED6D-ABC2-B749-B761-98A3ACF6E8B5}" name="Days completed" dataDxfId="104"/>
+    <tableColumn id="6" xr3:uid="{1E1A1903-5E63-2C42-A785-7622E4CE1FFD}" name="Progress" dataDxfId="103">
       <calculatedColumnFormula>Project_Data[[#This Row],[Days completed]]/Project_Data[[#This Row],[Duration]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5529251C-746B-0F49-8B21-221411C8E693}" name="Budget" dataDxfId="84"/>
-    <tableColumn id="8" xr3:uid="{2781FA1C-8107-3A45-8365-873CEB86F752}" name="Actual" dataDxfId="83"/>
+    <tableColumn id="7" xr3:uid="{5529251C-746B-0F49-8B21-221411C8E693}" name="Budget" dataDxfId="102"/>
+    <tableColumn id="8" xr3:uid="{2781FA1C-8107-3A45-8365-873CEB86F752}" name="Actual" dataDxfId="101"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7882,9 +8158,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18BA6329-E680-5548-BB82-D6FB67EB7003}">
   <dimension ref="A1:AA49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N15" sqref="N15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R54" sqref="R54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9178,7 +9454,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H9:H50">
-    <cfRule type="dataBar" priority="6">
+    <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -9192,22 +9468,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:Y8">
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="11" priority="6">
       <formula>$K8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:Y50">
-    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="2" stopIfTrue="1">
       <formula>AND(WEEKDAY(K$8,17)&gt;5, $B9&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>AND(K$8 &gt;= $D9, WORKDAY.INTL($D9, $G9, 7)-1 &gt;= K$8)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>AND(K$8 &gt;= WORKDAY.INTL($D9, $G9, 7), $H9 &lt;&gt; 1, K$8 &lt;= $E9)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="3" stopIfTrue="1">
       <formula>AND(K$8 &gt;= WORKDAY.INTL($D9, $G9, 7), $H9=0, K$8 &lt;= $E9)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="1">
+      <formula>$A9="Grand Total"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed formatting and completed dashboard
</commit_message>
<xml_diff>
--- a/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
+++ b/Excel Projects/Managing Multiple Project Progress/Multiple Project Progress Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafsanalmamun/Downloads/Data-Analysis_Data-Science_Projects/Excel Projects/Managing Multiple Project Progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1DFE96-F6A3-F34A-B9EC-D256F893F067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7476E8D5-E0E3-EE4A-9E98-F63C30FC01C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
+    <workbookView xWindow="-20" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{C2DE81AA-19AB-3641-B567-292C68886DC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="3" r:id="rId1"/>
@@ -6019,7 +6019,7 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8344,7 +8344,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U4" sqref="U4"/>
+      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>